<commit_message>
Update phone data-testid values
(cherry picked from commit a1cd3f82d2318f24cbe074d05c6e37590b9f6d87)
</commit_message>
<xml_diff>
--- a/test/e2e/List of data-testids.xlsx
+++ b/test/e2e/List of data-testids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\test\e2e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBAF2C1-0B70-4D88-A6FB-2B346DCC3661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7CCF5F-F9C8-42E6-891B-C3EC28E63849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2190" yWindow="1215" windowWidth="24330" windowHeight="12585" xr2:uid="{51F30F27-9EA9-4B4D-86A3-E32FA30758F4}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="267">
   <si>
     <t>Output</t>
   </si>
@@ -538,6 +538,9 @@
     <t>Range</t>
   </si>
   <si>
+    <t>save</t>
+  </si>
+  <si>
     <t>buffer_save</t>
   </si>
   <si>
@@ -719,6 +722,114 @@
   </si>
   <si>
     <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vue</t>
+  </si>
+  <si>
+    <t>isConnecting</t>
+  </si>
+  <si>
+    <t>isOnCall</t>
+  </si>
+  <si>
+    <t>isInboundCall</t>
+  </si>
+  <si>
+    <t>isOutboundCall</t>
+  </si>
+  <si>
+    <t>isCompleted</t>
+  </si>
+  <si>
+    <t>currentScriptHeader</t>
+  </si>
+  <si>
+    <t>currentScript.value</t>
+  </si>
+  <si>
+    <t>caller</t>
+  </si>
+  <si>
+    <t>caller.dnis</t>
+  </si>
+  <si>
+    <t>caller.location_name_state_name</t>
+  </si>
+  <si>
+    <t>number_of_inbound_calls</t>
+  </si>
+  <si>
+    <t>existing_cases</t>
+  </si>
+  <si>
+    <t>new_case</t>
+  </si>
+  <si>
+    <t>worktypeSVG</t>
+  </si>
+  <si>
+    <t>caseNumber</t>
+  </si>
+  <si>
+    <t>case_name</t>
+  </si>
+  <si>
+    <t>case_address_state</t>
+  </si>
+  <si>
+    <t>hangup</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\Agent.vue</t>
+  </si>
+  <si>
+    <t>currentUser.mobile</t>
+  </si>
+  <si>
+    <t>phoneDashboard.languages</t>
+  </si>
+  <si>
+    <t>language_edit</t>
+  </si>
+  <si>
+    <t>isNotTakingCalls</t>
+  </si>
+  <si>
+    <t>isNotOnCall</t>
+  </si>
+  <si>
+    <t>serve_outbound_calls</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\AgentStats.vue</t>
+  </si>
+  <si>
+    <t>inbound_count</t>
+  </si>
+  <si>
+    <t>outbound_count</t>
+  </si>
+  <si>
+    <t>total_login_time</t>
+  </si>
+  <si>
+    <t>total_call_time</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\EditAgentModal.vue</t>
+  </si>
+  <si>
+    <t>update_agent</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>languages</t>
   </si>
 </sst>
 </file>
@@ -1073,8 +1184,8 @@
   <dimension ref="A1:G501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B211" sqref="B211"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D245" sqref="D245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5167,7 +5278,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\locations\LocationTool.vuebuffer_save</v>
       </c>
       <c r="D152" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E152" t="s">
         <v>15</v>
@@ -5194,7 +5305,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\locations\LocationTool.vueadd_poly</v>
       </c>
       <c r="D153" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E153" t="s">
         <v>15</v>
@@ -5221,7 +5332,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\locations\LocationTool.vuesubtract_poly</v>
       </c>
       <c r="D154" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E154" t="s">
         <v>15</v>
@@ -5237,7 +5348,7 @@
     </row>
     <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B155" t="str">
         <f t="shared" si="9"/>
@@ -5265,7 +5376,7 @@
     </row>
     <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B156" t="str">
         <f t="shared" si="9"/>
@@ -5276,7 +5387,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuechange_organization</v>
       </c>
       <c r="D156" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E156" t="s">
         <v>69</v>
@@ -5292,7 +5403,7 @@
     </row>
     <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B157" t="str">
         <f t="shared" si="9"/>
@@ -5303,7 +5414,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuewhere_move_to</v>
       </c>
       <c r="D157" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E157" t="s">
         <v>92</v>
@@ -5319,7 +5430,7 @@
     </row>
     <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B158" t="str">
         <f t="shared" si="9"/>
@@ -5330,10 +5441,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuemove_new_organization</v>
       </c>
       <c r="D158" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E158" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F158" t="str">
         <f t="shared" si="12"/>
@@ -5346,7 +5457,7 @@
     </row>
     <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B159" t="str">
         <f t="shared" si="9"/>
@@ -5357,7 +5468,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuemove_new_organization</v>
       </c>
       <c r="D159" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E159" t="s">
         <v>93</v>
@@ -5373,7 +5484,7 @@
     </row>
     <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B160" t="str">
         <f t="shared" si="9"/>
@@ -5384,7 +5495,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuemove_existing_organization</v>
       </c>
       <c r="D160" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E160" t="s">
         <v>69</v>
@@ -5400,7 +5511,7 @@
     </row>
     <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B161" t="str">
         <f t="shared" si="9"/>
@@ -5411,7 +5522,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuemove_existing_organization</v>
       </c>
       <c r="D161" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E161" t="s">
         <v>93</v>
@@ -5427,7 +5538,7 @@
     </row>
     <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B162" t="str">
         <f t="shared" si="9"/>
@@ -5438,7 +5549,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueplease_select_target_organization</v>
       </c>
       <c r="D162" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E162" t="s">
         <v>69</v>
@@ -5454,7 +5565,7 @@
     </row>
     <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B163" t="str">
         <f t="shared" si="9"/>
@@ -5465,7 +5576,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueselect_organization_tab</v>
       </c>
       <c r="D163" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E163" t="s">
         <v>69</v>
@@ -5481,7 +5592,7 @@
     </row>
     <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B164" t="str">
         <f t="shared" si="9"/>
@@ -5492,7 +5603,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueselectedOrganization</v>
       </c>
       <c r="D164" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E164" t="s">
         <v>87</v>
@@ -5508,7 +5619,7 @@
     </row>
     <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B165" t="str">
         <f t="shared" si="9"/>
@@ -5519,7 +5630,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueselect_users_tab</v>
       </c>
       <c r="D165" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E165" t="s">
         <v>69</v>
@@ -5535,7 +5646,7 @@
     </row>
     <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B166" t="str">
         <f t="shared" si="9"/>
@@ -5546,7 +5657,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueselect_all_users</v>
       </c>
       <c r="D166" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E166" t="s">
         <v>66</v>
@@ -5562,7 +5673,7 @@
     </row>
     <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B167" t="str">
         <f t="shared" si="9"/>
@@ -5573,10 +5684,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuenestedUsers</v>
       </c>
       <c r="D167" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E167" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F167" t="str">
         <f t="shared" si="12"/>
@@ -5589,7 +5700,7 @@
     </row>
     <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B168" t="str">
         <f t="shared" si="9"/>
@@ -5600,7 +5711,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueselect_cases_tab</v>
       </c>
       <c r="D168" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E168" t="s">
         <v>69</v>
@@ -5616,7 +5727,7 @@
     </row>
     <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B169" t="str">
         <f t="shared" si="9"/>
@@ -5627,7 +5738,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueclaimedCases</v>
       </c>
       <c r="D169" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E169" t="s">
         <v>69</v>
@@ -5643,7 +5754,7 @@
     </row>
     <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B170" t="str">
         <f t="shared" si="9"/>
@@ -5670,7 +5781,7 @@
     </row>
     <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B171" t="str">
         <f t="shared" si="9"/>
@@ -5681,7 +5792,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueselect_all_cases</v>
       </c>
       <c r="D171" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E171" t="s">
         <v>66</v>
@@ -5697,7 +5808,7 @@
     </row>
     <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B172" t="str">
         <f t="shared" si="9"/>
@@ -5708,7 +5819,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuework_type</v>
       </c>
       <c r="D172" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E172" t="s">
         <v>69</v>
@@ -5724,7 +5835,7 @@
     </row>
     <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B173" t="str">
         <f t="shared" si="9"/>
@@ -5735,7 +5846,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuework_type</v>
       </c>
       <c r="D173" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E173" t="s">
         <v>66</v>
@@ -5751,7 +5862,7 @@
     </row>
     <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B174" t="str">
         <f t="shared" si="9"/>
@@ -5778,7 +5889,7 @@
     </row>
     <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B175" t="str">
         <f t="shared" si="9"/>
@@ -5789,7 +5900,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueback</v>
       </c>
       <c r="D175" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E175" t="s">
         <v>91</v>
@@ -5805,7 +5916,7 @@
     </row>
     <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B176" t="str">
         <f t="shared" si="9"/>
@@ -5816,7 +5927,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuenext</v>
       </c>
       <c r="D176" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E176" t="s">
         <v>91</v>
@@ -5832,7 +5943,7 @@
     </row>
     <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B177" t="str">
         <f t="shared" si="9"/>
@@ -5843,7 +5954,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vuemove</v>
       </c>
       <c r="D177" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E177" t="s">
         <v>15</v>
@@ -5859,7 +5970,7 @@
     </row>
     <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B178" t="str">
         <f t="shared" si="9"/>
@@ -5870,7 +5981,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ChangeOrganizationModal.vueOrganizationSearchInput</v>
       </c>
       <c r="D178" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E178" t="s">
         <v>87</v>
@@ -5886,7 +5997,7 @@
     </row>
     <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B179" t="str">
         <f t="shared" si="9"/>
@@ -5897,7 +6008,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\CompletedTransferModal.vueyou_have_been_moved</v>
       </c>
       <c r="D179" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E179" t="s">
         <v>98</v>
@@ -5913,7 +6024,7 @@
     </row>
     <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B180" t="str">
         <f t="shared" si="9"/>
@@ -5924,7 +6035,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\CompletedTransferModal.vueyou_have_been_moved_to</v>
       </c>
       <c r="D180" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E180" t="s">
         <v>69</v>
@@ -5940,7 +6051,7 @@
     </row>
     <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B181" t="str">
         <f t="shared" si="9"/>
@@ -5951,7 +6062,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\CompletedTransferModal.vuemove_back</v>
       </c>
       <c r="D181" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E181" t="s">
         <v>15</v>
@@ -5967,7 +6078,7 @@
     </row>
     <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B182" t="str">
         <f t="shared" si="9"/>
@@ -5978,7 +6089,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\CompletedTransferModal.vuestay</v>
       </c>
       <c r="D182" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E182" t="s">
         <v>15</v>
@@ -5994,7 +6105,7 @@
     </row>
     <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B183" t="str">
         <f t="shared" si="9"/>
@@ -6005,7 +6116,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\InviteUsers.vueinvite_new_user</v>
       </c>
       <c r="D183" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E183" t="s">
         <v>15</v>
@@ -6021,7 +6132,7 @@
     </row>
     <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B184" t="str">
         <f t="shared" si="9"/>
@@ -6032,7 +6143,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\InviteUsers.vueinvite_user</v>
       </c>
       <c r="D184" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E184" t="s">
         <v>98</v>
@@ -6048,7 +6159,7 @@
     </row>
     <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B185" t="str">
         <f t="shared" si="9"/>
@@ -6059,7 +6170,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\InviteUsers.vueinvite_teammates_instructions</v>
       </c>
       <c r="D185" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E185" t="s">
         <v>69</v>
@@ -6075,7 +6186,7 @@
     </row>
     <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B186" t="str">
         <f t="shared" si="9"/>
@@ -6086,7 +6197,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\InviteUsers.vueuserEmailsToInvite</v>
       </c>
       <c r="D186" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E186" t="s">
         <v>68</v>
@@ -6102,7 +6213,7 @@
     </row>
     <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B187" t="str">
         <f t="shared" si="9"/>
@@ -6113,7 +6224,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\InviteUsers.vueOrganizationSearch</v>
       </c>
       <c r="D187" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E187" t="s">
         <v>68</v>
@@ -6129,7 +6240,7 @@
     </row>
     <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B188" t="str">
         <f t="shared" si="9"/>
@@ -6156,7 +6267,7 @@
     </row>
     <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B189" t="str">
         <f t="shared" si="9"/>
@@ -6167,7 +6278,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\InviteUsers.vuesubmit_invites</v>
       </c>
       <c r="D189" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E189" t="s">
         <v>15</v>
@@ -6183,7 +6294,7 @@
     </row>
     <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B190" t="str">
         <f t="shared" si="9"/>
@@ -6194,7 +6305,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\RedeployRequest.vuerequest_redeploy</v>
       </c>
       <c r="D190" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E190" t="s">
         <v>15</v>
@@ -6210,7 +6321,7 @@
     </row>
     <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B191" t="str">
         <f t="shared" si="9"/>
@@ -6221,7 +6332,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\RedeployRequest.vueshowRedeploy</v>
       </c>
       <c r="D191" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E191" t="s">
         <v>98</v>
@@ -6237,7 +6348,7 @@
     </row>
     <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B192" t="str">
         <f t="shared" si="9"/>
@@ -6248,7 +6359,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\RedeployRequest.vuechoose_an_incident</v>
       </c>
       <c r="D192" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E192" t="s">
         <v>69</v>
@@ -6264,7 +6375,7 @@
     </row>
     <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B193" t="str">
         <f t="shared" si="9"/>
@@ -6275,7 +6386,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\RedeployRequest.vueselect_incident</v>
       </c>
       <c r="D193" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E193" t="s">
         <v>87</v>
@@ -6291,7 +6402,7 @@
     </row>
     <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B194" t="str">
         <f t="shared" si="9"/>
@@ -6318,7 +6429,7 @@
     </row>
     <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B195" t="str">
         <f t="shared" si="9"/>
@@ -6329,7 +6440,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\RedeployRequest.vuesubmit</v>
       </c>
       <c r="D195" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E195" t="s">
         <v>15</v>
@@ -6343,9 +6454,9 @@
         <v>data-testid="testSubmitButton"</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B196" t="str">
         <f t="shared" ref="B196:B259" si="13">IF(A196="","",MID(A196,FIND("@",SUBSTITUTE(A196,"\","@",LEN(A196)-LEN(SUBSTITUTE(A196,"\",""))))+1,LEN(A196)))</f>
@@ -6356,7 +6467,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ShareWorksite.vuemanually_enter_emails</v>
       </c>
       <c r="D196" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E196" t="s">
         <v>68</v>
@@ -6370,9 +6481,9 @@
         <v>data-testid="testManuallyEnterEmailsTextInput"</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B197" t="str">
         <f t="shared" si="13"/>
@@ -6383,10 +6494,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ShareWorksite.vuesearch_emails</v>
       </c>
       <c r="D197" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E197" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F197" t="str">
         <f t="shared" si="12"/>
@@ -6397,9 +6508,9 @@
         <v>data-testid="testSearchEmailsSearch"</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B198" t="str">
         <f t="shared" si="13"/>
@@ -6410,7 +6521,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ShareWorksite.vuemanually_enter_phones</v>
       </c>
       <c r="D198" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E198" t="s">
         <v>68</v>
@@ -6424,9 +6535,9 @@
         <v>data-testid="testManuallyEnterPhonesTextInput"</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B199" t="str">
         <f t="shared" si="13"/>
@@ -6437,10 +6548,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ShareWorksite.vuesearch_phones</v>
       </c>
       <c r="D199" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E199" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F199" t="str">
         <f t="shared" si="12"/>
@@ -6451,9 +6562,9 @@
         <v>data-testid="testSearchPhonesSearch"</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B200" t="str">
         <f t="shared" si="13"/>
@@ -6464,7 +6575,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\ShareWorksite.vueadd_message_to_invite</v>
       </c>
       <c r="D200" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E200" t="s">
         <v>67</v>
@@ -6478,9 +6589,9 @@
         <v>data-testid="testAddMessageToInviteTextarea"</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B201" t="str">
         <f t="shared" si="13"/>
@@ -6491,7 +6602,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\TermsandConditionsModal.vueterms_conditions_title</v>
       </c>
       <c r="D201" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E201" t="s">
         <v>98</v>
@@ -6505,9 +6616,9 @@
         <v>data-testid="testTermsConditionsTitleModal"</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B202" t="str">
         <f t="shared" si="13"/>
@@ -6518,7 +6629,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\modals\TermsandConditionsModal.vuetermsmodal.accept</v>
       </c>
       <c r="D202" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E202" t="s">
         <v>15</v>
@@ -6532,9 +6643,9 @@
         <v>data-testid="testTermsmodalAcceptButton"</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B203" t="str">
         <f t="shared" si="13"/>
@@ -6545,7 +6656,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\navigation\NavButton.vuenewBadge</v>
       </c>
       <c r="D203" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E203" t="s">
         <v>93</v>
@@ -6559,9 +6670,9 @@
         <v>data-testid="testNewBadgeIcon"</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B204" t="str">
         <f t="shared" si="13"/>
@@ -6587,9 +6698,9 @@
         <v>data-testid="test:SeveralCalculated"</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B205" t="str">
         <f t="shared" si="13"/>
@@ -6615,9 +6726,9 @@
         <v>data-testid="test:SeveralCalculated"</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B206" t="str">
         <f t="shared" si="13"/>
@@ -6628,7 +6739,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\navigation\NavMenu.vuecrisiscleanup_logo</v>
       </c>
       <c r="D206" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E206" t="s">
         <v>93</v>
@@ -6642,9 +6753,9 @@
         <v>data-testid="testCrisiscleanupLogoIcon"</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B207" t="str">
         <f t="shared" si="13"/>
@@ -6655,7 +6766,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\navigation\PewPewNavBar.vuepew_pew_logo</v>
       </c>
       <c r="D207" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E207" t="s">
         <v>93</v>
@@ -6669,9 +6780,9 @@
         <v>data-testid="testPewPewLogoIcon"</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B208" t="str">
         <f t="shared" si="13"/>
@@ -6682,7 +6793,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\navigation\PewPewNavBar.vuecrisiscleanup_logo</v>
       </c>
       <c r="D208" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E208" t="s">
         <v>93</v>
@@ -6696,9 +6807,9 @@
         <v>data-testid="testCrisiscleanupLogoIcon"</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B209" t="str">
         <f t="shared" si="13"/>
@@ -6724,9 +6835,9 @@
         <v>data-testid="test:SeveralCalculated"</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B210" t="str">
         <f t="shared" si="13"/>
@@ -6737,7 +6848,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\navigation\PewPewNavBar.vueregister</v>
       </c>
       <c r="D210" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E210" t="s">
         <v>15</v>
@@ -6751,865 +6862,1021 @@
         <v>data-testid="testRegisterButton"</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B211" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C211" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E211" t="str">
-        <f>IF(COUNTIF(C$2:C210,C211)&gt;0,"Button","")</f>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vueisConnecting</v>
+      </c>
+      <c r="D211" t="s">
+        <v>232</v>
+      </c>
+      <c r="E211" t="s">
+        <v>69</v>
       </c>
       <c r="F211" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testIsConnectingDiv</v>
       </c>
       <c r="G211" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIsConnectingDiv"</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B212" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C212" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E212" t="str">
-        <f>IF(COUNTIF(C$2:C211,C212)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vueisOnCall</v>
+      </c>
+      <c r="D212" t="s">
+        <v>233</v>
+      </c>
+      <c r="E212" t="s">
+        <v>69</v>
       </c>
       <c r="F212" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testIsOnCallDiv</v>
       </c>
       <c r="G212" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIsOnCallDiv"</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B213" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C213" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E213" t="str">
-        <f>IF(COUNTIF(C$2:C212,C213)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vueisInboundCall</v>
+      </c>
+      <c r="D213" t="s">
+        <v>234</v>
+      </c>
+      <c r="E213" t="s">
+        <v>69</v>
       </c>
       <c r="F213" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testIsInboundCallDiv</v>
       </c>
       <c r="G213" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIsInboundCallDiv"</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B214" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C214" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E214" t="str">
-        <f>IF(COUNTIF(C$2:C213,C214)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vueisOutboundCall</v>
+      </c>
+      <c r="D214" t="s">
+        <v>235</v>
+      </c>
+      <c r="E214" t="s">
+        <v>69</v>
       </c>
       <c r="F214" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testIsOutboundCallDiv</v>
       </c>
       <c r="G214" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIsOutboundCallDiv"</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B215" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C215" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E215" t="str">
-        <f>IF(COUNTIF(C$2:C214,C215)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vueisCompleted</v>
+      </c>
+      <c r="D215" t="s">
+        <v>236</v>
+      </c>
+      <c r="E215" t="s">
+        <v>69</v>
       </c>
       <c r="F215" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testIsCompletedDiv</v>
       </c>
       <c r="G215" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIsCompletedDiv"</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B216" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C216" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E216" t="str">
-        <f>IF(COUNTIF(C$2:C215,C216)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuecurrentScriptHeader</v>
+      </c>
+      <c r="D216" t="s">
+        <v>237</v>
+      </c>
+      <c r="E216" t="s">
+        <v>92</v>
       </c>
       <c r="F216" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testCurrentScriptHeaderContent</v>
       </c>
       <c r="G216" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCurrentScriptHeaderContent"</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B217" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C217" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E217" t="str">
-        <f>IF(COUNTIF(C$2:C216,C217)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuecurrentScript.value</v>
+      </c>
+      <c r="D217" t="s">
+        <v>238</v>
+      </c>
+      <c r="E217" t="s">
+        <v>92</v>
       </c>
       <c r="F217" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testCurrentScriptValueContent</v>
       </c>
       <c r="G217" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCurrentScriptValueContent"</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B218" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C218" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E218" t="str">
-        <f>IF(COUNTIF(C$2:C217,C218)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuecaller</v>
+      </c>
+      <c r="D218" t="s">
+        <v>239</v>
+      </c>
+      <c r="E218" t="s">
+        <v>69</v>
       </c>
       <c r="F218" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testCallerDiv</v>
       </c>
       <c r="G218" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCallerDiv"</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B219" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C219" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E219" t="str">
-        <f>IF(COUNTIF(C$2:C218,C219)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuecaller.dnis</v>
+      </c>
+      <c r="D219" t="s">
+        <v>240</v>
+      </c>
+      <c r="E219" t="s">
+        <v>92</v>
       </c>
       <c r="F219" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testCallerDnisContent</v>
       </c>
       <c r="G219" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCallerDnisContent"</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B220" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C220" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E220" t="str">
-        <f>IF(COUNTIF(C$2:C219,C220)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuecaller.location_name_state_name</v>
+      </c>
+      <c r="D220" t="s">
+        <v>241</v>
+      </c>
+      <c r="E220" t="s">
+        <v>92</v>
       </c>
       <c r="F220" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testCallerLocationNameStateNameContent</v>
       </c>
       <c r="G220" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCallerLocationNameStateNameContent"</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B221" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C221" t="str">
         <f t="shared" si="14"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
-      </c>
-      <c r="E221" t="str">
-        <f>IF(COUNTIF(C$2:C220,C221)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuenumber_of_inbound_calls</v>
+      </c>
+      <c r="D221" t="s">
+        <v>242</v>
+      </c>
+      <c r="E221" t="s">
+        <v>69</v>
       </c>
       <c r="F221" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testNumberOfInboundCallsDiv</v>
       </c>
       <c r="G221" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testNumberOfInboundCallsDiv"</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>231</v>
+      </c>
       <c r="B222" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C222" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E222" t="str">
-        <f>IF(COUNTIF(C$2:C221,C222)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vueexisting_cases</v>
+      </c>
+      <c r="D222" t="s">
+        <v>243</v>
+      </c>
+      <c r="E222" t="s">
+        <v>69</v>
       </c>
       <c r="F222" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testExistingCasesDiv</v>
       </c>
       <c r="G222" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testExistingCasesDiv"</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>231</v>
+      </c>
       <c r="B223" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C223" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E223" t="str">
-        <f>IF(COUNTIF(C$2:C222,C223)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuenew_case</v>
+      </c>
+      <c r="D223" t="s">
+        <v>244</v>
+      </c>
+      <c r="E223" t="s">
+        <v>92</v>
       </c>
       <c r="F223" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testNewCaseContent</v>
       </c>
       <c r="G223" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testNewCaseContent"</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>231</v>
+      </c>
       <c r="B224" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C224" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vue:several_calculated</v>
+      </c>
+      <c r="D224" t="s">
+        <v>104</v>
       </c>
       <c r="E224" t="str">
         <f>IF(COUNTIF(C$2:C223,C224)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F224" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>test:SeveralCalculated</v>
       </c>
       <c r="G224" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="225" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="test:SeveralCalculated"</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>231</v>
+      </c>
       <c r="B225" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C225" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E225" t="str">
-        <f>IF(COUNTIF(C$2:C224,C225)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vueworktypeSVG</v>
+      </c>
+      <c r="D225" t="s">
+        <v>245</v>
+      </c>
+      <c r="E225" t="s">
+        <v>93</v>
       </c>
       <c r="F225" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testWorktypeSVGIcon</v>
       </c>
       <c r="G225" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="226" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testWorktypeSVGIcon"</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>231</v>
+      </c>
       <c r="B226" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C226" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E226" t="str">
-        <f>IF(COUNTIF(C$2:C225,C226)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuecaseNumber</v>
+      </c>
+      <c r="D226" t="s">
+        <v>246</v>
+      </c>
+      <c r="E226" t="s">
+        <v>69</v>
       </c>
       <c r="F226" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testCaseNumberDiv</v>
       </c>
       <c r="G226" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="227" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCaseNumberDiv"</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>231</v>
+      </c>
       <c r="B227" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C227" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E227" t="str">
-        <f>IF(COUNTIF(C$2:C226,C227)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuecase_name</v>
+      </c>
+      <c r="D227" t="s">
+        <v>247</v>
+      </c>
+      <c r="E227" t="s">
+        <v>69</v>
       </c>
       <c r="F227" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testCaseNameDiv</v>
       </c>
       <c r="G227" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="228" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCaseNameDiv"</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>231</v>
+      </c>
       <c r="B228" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C228" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E228" t="str">
-        <f>IF(COUNTIF(C$2:C227,C228)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuecase_address_state</v>
+      </c>
+      <c r="D228" t="s">
+        <v>248</v>
+      </c>
+      <c r="E228" t="s">
+        <v>69</v>
       </c>
       <c r="F228" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testCaseAddressStateDiv</v>
       </c>
       <c r="G228" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="229" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCaseAddressStateDiv"</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>231</v>
+      </c>
       <c r="B229" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>ActiveCall.vue</v>
       </c>
       <c r="C229" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E229" t="str">
-        <f>IF(COUNTIF(C$2:C228,C229)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\ActiveCall.vuehangup</v>
+      </c>
+      <c r="D229" t="s">
+        <v>249</v>
+      </c>
+      <c r="E229" t="s">
+        <v>93</v>
       </c>
       <c r="F229" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testHangupIcon</v>
       </c>
       <c r="G229" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="230" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testHangupIcon"</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>250</v>
+      </c>
       <c r="B230" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>Agent.vue</v>
       </c>
       <c r="C230" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E230" t="str">
-        <f>IF(COUNTIF(C$2:C229,C230)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\Agent.vuecurrentUser.mobile</v>
+      </c>
+      <c r="D230" t="s">
+        <v>251</v>
+      </c>
+      <c r="E230" t="s">
+        <v>92</v>
       </c>
       <c r="F230" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testCurrentUserMobileContent</v>
       </c>
       <c r="G230" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="231" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCurrentUserMobileContent"</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>250</v>
+      </c>
       <c r="B231" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>Agent.vue</v>
       </c>
       <c r="C231" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E231" t="str">
-        <f>IF(COUNTIF(C$2:C230,C231)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\Agent.vuephoneDashboard.languages</v>
+      </c>
+      <c r="D231" t="s">
+        <v>252</v>
+      </c>
+      <c r="E231" t="s">
+        <v>69</v>
       </c>
       <c r="F231" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testPhoneDashboardLanguagesDiv</v>
       </c>
       <c r="G231" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="232" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testPhoneDashboardLanguagesDiv"</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>250</v>
+      </c>
       <c r="B232" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>Agent.vue</v>
       </c>
       <c r="C232" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E232" t="str">
-        <f>IF(COUNTIF(C$2:C231,C232)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\Agent.vuelanguage_edit</v>
+      </c>
+      <c r="D232" t="s">
+        <v>253</v>
+      </c>
+      <c r="E232" t="s">
+        <v>93</v>
       </c>
       <c r="F232" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testLanguageEditIcon</v>
       </c>
       <c r="G232" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="233" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testLanguageEditIcon"</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>250</v>
+      </c>
       <c r="B233" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>Agent.vue</v>
       </c>
       <c r="C233" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E233" t="str">
-        <f>IF(COUNTIF(C$2:C232,C233)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\Agent.vueisOnCall</v>
+      </c>
+      <c r="D233" t="s">
+        <v>233</v>
+      </c>
+      <c r="E233" t="s">
+        <v>15</v>
       </c>
       <c r="F233" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testIsOnCallButton</v>
       </c>
       <c r="G233" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="234" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIsOnCallButton"</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>250</v>
+      </c>
       <c r="B234" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>Agent.vue</v>
       </c>
       <c r="C234" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E234" t="str">
-        <f>IF(COUNTIF(C$2:C233,C234)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\Agent.vueisNotTakingCalls</v>
+      </c>
+      <c r="D234" t="s">
+        <v>254</v>
+      </c>
+      <c r="E234" t="s">
+        <v>15</v>
       </c>
       <c r="F234" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testIsNotTakingCallsButton</v>
       </c>
       <c r="G234" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="235" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIsNotTakingCallsButton"</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>250</v>
+      </c>
       <c r="B235" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>Agent.vue</v>
       </c>
       <c r="C235" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E235" t="str">
-        <f>IF(COUNTIF(C$2:C234,C235)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\Agent.vueisNotOnCall</v>
+      </c>
+      <c r="D235" t="s">
+        <v>255</v>
+      </c>
+      <c r="E235" t="s">
+        <v>15</v>
       </c>
       <c r="F235" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testIsNotOnCallButton</v>
       </c>
       <c r="G235" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="236" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIsNotOnCallButton"</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>250</v>
+      </c>
       <c r="B236" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>Agent.vue</v>
       </c>
       <c r="C236" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E236" t="str">
-        <f>IF(COUNTIF(C$2:C235,C236)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\Agent.vueserve_outbound_calls</v>
+      </c>
+      <c r="D236" t="s">
+        <v>256</v>
+      </c>
+      <c r="E236" t="s">
+        <v>66</v>
       </c>
       <c r="F236" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testServeOutboundCallsCheckbox</v>
       </c>
       <c r="G236" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="237" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testServeOutboundCallsCheckbox"</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>250</v>
+      </c>
       <c r="B237" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>Agent.vue</v>
       </c>
       <c r="C237" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E237" t="str">
-        <f>IF(COUNTIF(C$2:C236,C237)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\Agent.vuehangup</v>
+      </c>
+      <c r="D237" t="s">
+        <v>249</v>
+      </c>
+      <c r="E237" t="s">
+        <v>93</v>
       </c>
       <c r="F237" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testHangupIcon</v>
       </c>
       <c r="G237" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="238" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testHangupIcon"</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>257</v>
+      </c>
       <c r="B238" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>AgentStats.vue</v>
       </c>
       <c r="C238" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E238" t="str">
-        <f>IF(COUNTIF(C$2:C237,C238)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\AgentStats.vueinbound_count</v>
+      </c>
+      <c r="D238" t="s">
+        <v>258</v>
+      </c>
+      <c r="E238" t="s">
+        <v>69</v>
       </c>
       <c r="F238" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testInboundCountDiv</v>
       </c>
       <c r="G238" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="239" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testInboundCountDiv"</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>257</v>
+      </c>
       <c r="B239" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>AgentStats.vue</v>
       </c>
       <c r="C239" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E239" t="str">
-        <f>IF(COUNTIF(C$2:C238,C239)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\AgentStats.vueoutbound_count</v>
+      </c>
+      <c r="D239" t="s">
+        <v>259</v>
+      </c>
+      <c r="E239" t="s">
+        <v>69</v>
       </c>
       <c r="F239" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testOutboundCountDiv</v>
       </c>
       <c r="G239" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="240" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testOutboundCountDiv"</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>257</v>
+      </c>
       <c r="B240" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>AgentStats.vue</v>
       </c>
       <c r="C240" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E240" t="str">
-        <f>IF(COUNTIF(C$2:C239,C240)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\AgentStats.vuetotal_login_time</v>
+      </c>
+      <c r="D240" t="s">
+        <v>260</v>
+      </c>
+      <c r="E240" t="s">
+        <v>69</v>
       </c>
       <c r="F240" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testTotalLoginTimeDiv</v>
       </c>
       <c r="G240" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="241" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testTotalLoginTimeDiv"</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>257</v>
+      </c>
       <c r="B241" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>AgentStats.vue</v>
       </c>
       <c r="C241" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E241" t="str">
-        <f>IF(COUNTIF(C$2:C240,C241)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\AgentStats.vuetotal_call_time</v>
+      </c>
+      <c r="D241" t="s">
+        <v>261</v>
+      </c>
+      <c r="E241" t="s">
+        <v>69</v>
       </c>
       <c r="F241" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testTotalCallTimeDiv</v>
       </c>
       <c r="G241" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="242" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testTotalCallTimeDiv"</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>262</v>
+      </c>
       <c r="B242" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>EditAgentModal.vue</v>
       </c>
       <c r="C242" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E242" t="str">
-        <f>IF(COUNTIF(C$2:C241,C242)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\EditAgentModal.vueupdate_agent</v>
+      </c>
+      <c r="D242" t="s">
+        <v>263</v>
+      </c>
+      <c r="E242" t="s">
+        <v>69</v>
       </c>
       <c r="F242" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testUpdateAgentDiv</v>
       </c>
       <c r="G242" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testUpdateAgentDiv"</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>230</v>
+      </c>
       <c r="B243" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C243" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E243" t="str">
-        <f>IF(COUNTIF(C$2:C242,C243)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\phone_number</v>
+      </c>
+      <c r="D243" t="s">
+        <v>264</v>
+      </c>
+      <c r="E243" t="s">
+        <v>92</v>
       </c>
       <c r="F243" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testPhoneNumberContent</v>
       </c>
       <c r="G243" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="244" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testPhoneNumberContent"</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>230</v>
+      </c>
       <c r="B244" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C244" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E244" t="str">
-        <f>IF(COUNTIF(C$2:C243,C244)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\phoneNumber</v>
+      </c>
+      <c r="D244" t="s">
+        <v>265</v>
+      </c>
+      <c r="E244" t="s">
+        <v>68</v>
       </c>
       <c r="F244" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testPhoneNumberTextInput</v>
       </c>
       <c r="G244" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testPhoneNumberTextInput"</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>230</v>
+      </c>
       <c r="B245" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C245" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E245" t="str">
-        <f>IF(COUNTIF(C$2:C244,C245)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\languages</v>
+      </c>
+      <c r="D245" t="s">
+        <v>266</v>
+      </c>
+      <c r="E245" t="s">
+        <v>92</v>
       </c>
       <c r="F245" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testLanguagesContent</v>
       </c>
       <c r="G245" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testLanguagesContent"</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>230</v>
+      </c>
       <c r="B246" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C246" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E246" t="str">
-        <f>IF(COUNTIF(C$2:C245,C246)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\languages</v>
+      </c>
+      <c r="D246" t="s">
+        <v>266</v>
+      </c>
+      <c r="E246" t="s">
+        <v>87</v>
       </c>
       <c r="F246" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testLanguagesSelect</v>
       </c>
       <c r="G246" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="247" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testLanguagesSelect"</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>230</v>
+      </c>
       <c r="B247" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C247" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="E247" t="str">
-        <f>IF(COUNTIF(C$2:C246,C247)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\save</v>
+      </c>
+      <c r="D247" t="s">
+        <v>169</v>
+      </c>
+      <c r="E247" t="s">
+        <v>15</v>
       </c>
       <c r="F247" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>testSaveButton</v>
       </c>
       <c r="G247" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSaveButton"</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>230</v>
+      </c>
       <c r="B248" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C248" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
       </c>
       <c r="E248" t="str">
         <f>IF(COUNTIF(C$2:C247,C248)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F248" t="str">
         <f t="shared" si="16"/>
@@ -7620,14 +7887,17 @@
         <v/>
       </c>
     </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>230</v>
+      </c>
       <c r="B249" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C249" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
       </c>
       <c r="E249" t="str">
         <f>IF(COUNTIF(C$2:C248,C249)&gt;0,"Button","")</f>
@@ -7642,14 +7912,17 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>230</v>
+      </c>
       <c r="B250" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C250" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
       </c>
       <c r="E250" t="str">
         <f>IF(COUNTIF(C$2:C249,C250)&gt;0,"Button","")</f>
@@ -7664,14 +7937,17 @@
         <v/>
       </c>
     </row>
-    <row r="251" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>230</v>
+      </c>
       <c r="B251" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C251" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
       </c>
       <c r="E251" t="str">
         <f>IF(COUNTIF(C$2:C250,C251)&gt;0,"Button","")</f>
@@ -7686,14 +7962,17 @@
         <v/>
       </c>
     </row>
-    <row r="252" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>230</v>
+      </c>
       <c r="B252" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C252" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
       </c>
       <c r="E252" t="str">
         <f>IF(COUNTIF(C$2:C251,C252)&gt;0,"Button","")</f>
@@ -7708,14 +7987,17 @@
         <v/>
       </c>
     </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>230</v>
+      </c>
       <c r="B253" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C253" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
       </c>
       <c r="E253" t="str">
         <f>IF(COUNTIF(C$2:C252,C253)&gt;0,"Button","")</f>
@@ -7730,14 +8012,17 @@
         <v/>
       </c>
     </row>
-    <row r="254" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>230</v>
+      </c>
       <c r="B254" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C254" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
       </c>
       <c r="E254" t="str">
         <f>IF(COUNTIF(C$2:C253,C254)&gt;0,"Button","")</f>
@@ -7752,14 +8037,17 @@
         <v/>
       </c>
     </row>
-    <row r="255" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>230</v>
+      </c>
       <c r="B255" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="C255" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\phone\</v>
       </c>
       <c r="E255" t="str">
         <f>IF(COUNTIF(C$2:C254,C255)&gt;0,"Button","")</f>
@@ -7774,7 +8062,7 @@
         <v/>
       </c>
     </row>
-    <row r="256" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B256" t="str">
         <f t="shared" si="13"/>
         <v/>
@@ -13306,12 +13594,12 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continue adding data-testids to \work
(cherry picked from commit 02dccaf6d9c6f513e6f923be03a967de7e61b4db)
</commit_message>
<xml_diff>
--- a/test/e2e/List of data-testids.xlsx
+++ b/test/e2e/List of data-testids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\test\e2e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AD488E-DD8E-4ABF-A378-69E3A9D65C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B57E00E-2220-475B-9C88-0CBA5F06381C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="510" windowWidth="24330" windowHeight="12585" xr2:uid="{51F30F27-9EA9-4B4D-86A3-E32FA30758F4}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="468">
   <si>
     <t>Output</t>
   </si>
@@ -1114,6 +1114,12 @@
     <t>case</t>
   </si>
   <si>
+    <t>member_of_my_org</t>
+  </si>
+  <si>
+    <t>isHighPriority</t>
+  </si>
+  <si>
     <t>is_not_member_of_my_org</t>
   </si>
   <si>
@@ -1274,6 +1280,159 @@
   </si>
   <si>
     <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vue</t>
+  </si>
+  <si>
+    <t>intake_form</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>phone1</t>
+  </si>
+  <si>
+    <t>phone2</t>
+  </si>
+  <si>
+    <t>add_phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>primary_language</t>
+  </si>
+  <si>
+    <t>auto_contact_frequency</t>
+  </si>
+  <si>
+    <t>location_instructions</t>
+  </si>
+  <si>
+    <t>clear_location</t>
+  </si>
+  <si>
+    <t>manually_edit_address</t>
+  </si>
+  <si>
+    <t>full_address</t>
+  </si>
+  <si>
+    <t>WorksiteSearchInput</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>what3words</t>
+  </si>
+  <si>
+    <t>use_my_location</t>
+  </si>
+  <si>
+    <t>toggleSelectOnMap</t>
+  </si>
+  <si>
+    <t>saveNote</t>
+  </si>
+  <si>
+    <t>address_problems</t>
+  </si>
+  <si>
+    <t>worksite.total_time</t>
+  </si>
+  <si>
+    <t>worksiteImageSection</t>
+  </si>
+  <si>
+    <t>save_claim</t>
+  </si>
+  <si>
+    <t>postal_code</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes.vue</t>
+  </si>
+  <si>
+    <t>worksite_notes</t>
+  </si>
+  <si>
+    <t>showAllNotes</t>
+  </si>
+  <si>
+    <t>showNotes</t>
+  </si>
+  <si>
+    <t>add_note</t>
+  </si>
+  <si>
+    <t>sticky_note</t>
+  </si>
+  <si>
+    <t>currentNote</t>
+  </si>
+  <si>
+    <t>cancelNote</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteReportSection.vue</t>
+  </si>
+  <si>
+    <t>volunteersToAdd</t>
+  </si>
+  <si>
+    <t>hoursPerVolunteer</t>
+  </si>
+  <si>
+    <t>addTime</t>
+  </si>
+  <si>
+    <t>total_volunteers</t>
+  </si>
+  <si>
+    <t>currentTimeEdit</t>
+  </si>
+  <si>
+    <t>currentTimeSave</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteSearchInput.vue</t>
+  </si>
+  <si>
+    <t>worsiteSearchResults</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteTable.vue</t>
+  </si>
+  <si>
+    <t>worksiteTable</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteView.vue</t>
+  </si>
+  <si>
+    <t>worksiteFormContent</t>
+  </si>
+  <si>
+    <t>WorksiteNotes</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>call_number</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>claim_all</t>
   </si>
 </sst>
 </file>
@@ -1629,7 +1788,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A410" sqref="A410"/>
+      <selection pane="bottomLeft" activeCell="D466" sqref="D466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10912,7 +11071,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vueis_not_member_of_my_org</v>
       </c>
       <c r="D344" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E344" t="s">
         <v>93</v>
@@ -10939,7 +11098,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vueis_member_of_my_org</v>
       </c>
       <c r="D345" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="E345" t="s">
         <v>93</v>
@@ -10966,7 +11125,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vueis_high_priority</v>
       </c>
       <c r="D346" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E346" t="s">
         <v>93</v>
@@ -10993,7 +11152,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vueis_not_high_priority</v>
       </c>
       <c r="D347" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E347" t="s">
         <v>93</v>
@@ -11047,7 +11206,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vuejump_to_case</v>
       </c>
       <c r="D349" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="E349" t="s">
         <v>93</v>
@@ -11074,7 +11233,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vuehistory</v>
       </c>
       <c r="D350" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E350" t="s">
         <v>93</v>
@@ -11101,7 +11260,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vuedownload</v>
       </c>
       <c r="D351" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E351" t="s">
         <v>93</v>
@@ -11128,7 +11287,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vueshare</v>
       </c>
       <c r="D352" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="E352" t="s">
         <v>93</v>
@@ -11155,7 +11314,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vueprint</v>
       </c>
       <c r="D353" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E353" t="s">
         <v>93</v>
@@ -11182,7 +11341,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHeader.vueedit</v>
       </c>
       <c r="D354" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E354" t="s">
         <v>93</v>
@@ -11225,7 +11384,7 @@
     </row>
     <row r="356" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B356" t="str">
         <f t="shared" si="21"/>
@@ -11236,7 +11395,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHistory.vuecaseHistory</v>
       </c>
       <c r="D356" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E356" t="s">
         <v>69</v>
@@ -11252,7 +11411,7 @@
     </row>
     <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B357" t="str">
         <f t="shared" si="21"/>
@@ -11263,7 +11422,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\CaseHistory.vuedo_not_share_contact_warning</v>
       </c>
       <c r="D357" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E357" t="s">
         <v>69</v>
@@ -11279,7 +11438,7 @@
     </row>
     <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B358" t="str">
         <f t="shared" si="21"/>
@@ -11290,7 +11449,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\SectionHeading.vuehelp</v>
       </c>
       <c r="D358" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E358" t="s">
         <v>99</v>
@@ -11306,7 +11465,7 @@
     </row>
     <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B359" t="str">
         <f t="shared" si="21"/>
@@ -11317,7 +11476,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vuepda_heatmap</v>
       </c>
       <c r="D359" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E359" t="s">
         <v>66</v>
@@ -11333,7 +11492,7 @@
     </row>
     <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B360" t="str">
         <f t="shared" si="21"/>
@@ -11344,7 +11503,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vuepda_heatmap</v>
       </c>
       <c r="D360" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E360" t="s">
         <v>93</v>
@@ -11360,7 +11519,7 @@
     </row>
     <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B361" t="str">
         <f t="shared" si="21"/>
@@ -11371,7 +11530,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vuelayers</v>
       </c>
       <c r="D361" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="E361" t="s">
         <v>15</v>
@@ -11387,7 +11546,7 @@
     </row>
     <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B362" t="str">
         <f t="shared" si="21"/>
@@ -11398,7 +11557,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vueboundary_political_us_state</v>
       </c>
       <c r="D362" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E362" t="s">
         <v>69</v>
@@ -11414,7 +11573,7 @@
     </row>
     <row r="363" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B363" t="str">
         <f t="shared" si="21"/>
@@ -11425,7 +11584,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vueboundary_political_us_state</v>
       </c>
       <c r="D363" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E363" t="s">
         <v>66</v>
@@ -11441,7 +11600,7 @@
     </row>
     <row r="364" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B364" t="str">
         <f t="shared" si="21"/>
@@ -11452,7 +11611,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vueboundary_political_us_congress</v>
       </c>
       <c r="D364" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E364" t="s">
         <v>69</v>
@@ -11468,7 +11627,7 @@
     </row>
     <row r="365" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B365" t="str">
         <f t="shared" si="21"/>
@@ -11479,7 +11638,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vueboundary_political_us_congress</v>
       </c>
       <c r="D365" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E365" t="s">
         <v>66</v>
@@ -11495,7 +11654,7 @@
     </row>
     <row r="366" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B366" t="str">
         <f t="shared" si="21"/>
@@ -11506,7 +11665,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vueboundary_political_us_county</v>
       </c>
       <c r="D366" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E366" t="s">
         <v>69</v>
@@ -11522,7 +11681,7 @@
     </row>
     <row r="367" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B367" t="str">
         <f t="shared" si="21"/>
@@ -11533,7 +11692,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vueboundary_political_us_county</v>
       </c>
       <c r="D367" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E367" t="s">
         <v>66</v>
@@ -11549,7 +11708,7 @@
     </row>
     <row r="368" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B368" t="str">
         <f t="shared" si="21"/>
@@ -11576,7 +11735,7 @@
     </row>
     <row r="369" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B369" t="str">
         <f t="shared" si="21"/>
@@ -11603,7 +11762,7 @@
     </row>
     <row r="370" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B370" t="str">
         <f t="shared" si="21"/>
@@ -11614,7 +11773,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vueprimary_response_area</v>
       </c>
       <c r="D370" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="E370" t="s">
         <v>66</v>
@@ -11630,7 +11789,7 @@
     </row>
     <row r="371" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B371" t="str">
         <f t="shared" si="21"/>
@@ -11641,7 +11800,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vuesecondary_response_area</v>
       </c>
       <c r="D371" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E371" t="s">
         <v>66</v>
@@ -11657,7 +11816,7 @@
     </row>
     <row r="372" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B372" t="str">
         <f t="shared" si="21"/>
@@ -11668,7 +11827,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vuefilters</v>
       </c>
       <c r="D372" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E372" t="s">
         <v>15</v>
@@ -11684,7 +11843,7 @@
     </row>
     <row r="373" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B373" t="str">
         <f t="shared" si="21"/>
@@ -11695,7 +11854,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vueWorksiteFilters</v>
       </c>
       <c r="D373" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E373" t="s">
         <v>15</v>
@@ -11711,7 +11870,7 @@
     </row>
     <row r="374" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B374" t="str">
         <f t="shared" si="21"/>
@@ -11722,7 +11881,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteActions.vuedownload_csv</v>
       </c>
       <c r="D374" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E374" t="s">
         <v>15</v>
@@ -11738,7 +11897,7 @@
     </row>
     <row r="375" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B375" t="str">
         <f t="shared" si="21"/>
@@ -11749,7 +11908,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuefilters</v>
       </c>
       <c r="D375" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E375" t="s">
         <v>98</v>
@@ -11765,7 +11924,7 @@
     </row>
     <row r="376" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B376" t="str">
         <f t="shared" si="21"/>
@@ -11789,7 +11948,7 @@
     </row>
     <row r="377" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B377" t="str">
         <f t="shared" si="21"/>
@@ -11800,7 +11959,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueclear_filters</v>
       </c>
       <c r="D377" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="E377" t="s">
         <v>15</v>
@@ -11816,7 +11975,7 @@
     </row>
     <row r="378" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B378" t="str">
         <f t="shared" si="21"/>
@@ -11827,7 +11986,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuegeneralSection</v>
       </c>
       <c r="D378" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E378" t="s">
         <v>69</v>
@@ -11843,7 +12002,7 @@
     </row>
     <row r="379" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B379" t="str">
         <f t="shared" si="21"/>
@@ -11854,7 +12013,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuepersonalSection</v>
       </c>
       <c r="D379" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E379" t="s">
         <v>69</v>
@@ -11870,7 +12029,7 @@
     </row>
     <row r="380" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B380" t="str">
         <f t="shared" si="21"/>
@@ -11881,7 +12040,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueflagsSection</v>
       </c>
       <c r="D380" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E380" t="s">
         <v>69</v>
@@ -11897,7 +12056,7 @@
     </row>
     <row r="381" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B381" t="str">
         <f t="shared" si="21"/>
@@ -11908,7 +12067,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueworkSection</v>
       </c>
       <c r="D381" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E381" t="s">
         <v>69</v>
@@ -11924,7 +12083,7 @@
     </row>
     <row r="382" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B382" t="str">
         <f t="shared" si="21"/>
@@ -11935,7 +12094,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueteamsSection</v>
       </c>
       <c r="D382" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E382" t="s">
         <v>69</v>
@@ -11951,7 +12110,7 @@
     </row>
     <row r="383" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B383" t="str">
         <f t="shared" si="21"/>
@@ -11962,7 +12121,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuelocationsSection</v>
       </c>
       <c r="D383" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E383" t="s">
         <v>69</v>
@@ -11978,7 +12137,7 @@
     </row>
     <row r="384" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B384" t="str">
         <f t="shared" si="21"/>
@@ -11989,7 +12148,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuedateSection</v>
       </c>
       <c r="D384" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E384" t="s">
         <v>69</v>
@@ -12005,7 +12164,7 @@
     </row>
     <row r="385" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B385" t="str">
         <f t="shared" si="21"/>
@@ -12016,7 +12175,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueorganization_primary_location</v>
       </c>
       <c r="D385" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E385" t="s">
         <v>66</v>
@@ -12032,7 +12191,7 @@
     </row>
     <row r="386" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B386" t="str">
         <f t="shared" si="21"/>
@@ -12043,7 +12202,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueorganization_secondary_location</v>
       </c>
       <c r="D386" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E386" t="s">
         <v>66</v>
@@ -12059,7 +12218,7 @@
     </row>
     <row r="387" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B387" t="str">
         <f t="shared" si="21"/>
@@ -12070,7 +12229,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuemy_team</v>
       </c>
       <c r="D387" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E387" t="s">
         <v>66</v>
@@ -12086,7 +12245,7 @@
     </row>
     <row r="388" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B388" t="str">
         <f t="shared" ref="B388:B451" si="25">IF(A388="","",MID(A388,FIND("@",SUBSTITUTE(A388,"\","@",LEN(A388)-LEN(SUBSTITUTE(A388,"\",""))))+1,LEN(A388)))</f>
@@ -12097,7 +12256,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueunclaimed</v>
       </c>
       <c r="D388" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E388" t="s">
         <v>66</v>
@@ -12113,7 +12272,7 @@
     </row>
     <row r="389" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B389" t="str">
         <f t="shared" si="25"/>
@@ -12124,7 +12283,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueclaimed_by_org</v>
       </c>
       <c r="D389" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E389" t="s">
         <v>66</v>
@@ -12140,7 +12299,7 @@
     </row>
     <row r="390" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B390" t="str">
         <f t="shared" si="25"/>
@@ -12151,7 +12310,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuereported_by_org</v>
       </c>
       <c r="D390" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E390" t="s">
         <v>66</v>
@@ -12167,7 +12326,7 @@
     </row>
     <row r="391" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B391" t="str">
         <f t="shared" si="25"/>
@@ -12178,7 +12337,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueopen</v>
       </c>
       <c r="D391" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E391" t="s">
         <v>66</v>
@@ -12194,7 +12353,7 @@
     </row>
     <row r="392" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B392" t="str">
         <f t="shared" si="25"/>
@@ -12205,7 +12364,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueclosed</v>
       </c>
       <c r="D392" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="E392" t="s">
         <v>66</v>
@@ -12221,7 +12380,7 @@
     </row>
     <row r="393" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B393" t="str">
         <f t="shared" si="25"/>
@@ -12245,7 +12404,7 @@
     </row>
     <row r="394" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B394" t="str">
         <f t="shared" si="25"/>
@@ -12256,7 +12415,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueflags</v>
       </c>
       <c r="D394" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E394" t="s">
         <v>66</v>
@@ -12272,7 +12431,7 @@
     </row>
     <row r="395" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B395" t="str">
         <f t="shared" si="25"/>
@@ -12283,7 +12442,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuemember_of_my_organization</v>
       </c>
       <c r="D395" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E395" t="s">
         <v>66</v>
@@ -12299,7 +12458,7 @@
     </row>
     <row r="396" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B396" t="str">
         <f t="shared" si="25"/>
@@ -12323,7 +12482,7 @@
     </row>
     <row r="397" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B397" t="str">
         <f t="shared" si="25"/>
@@ -12334,7 +12493,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuemissing_work_type</v>
       </c>
       <c r="D397" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="E397" t="s">
         <v>66</v>
@@ -12350,7 +12509,7 @@
     </row>
     <row r="398" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B398" t="str">
         <f t="shared" si="25"/>
@@ -12374,7 +12533,7 @@
     </row>
     <row r="399" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B399" t="str">
         <f t="shared" si="25"/>
@@ -12385,7 +12544,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueorganization_primary_location2</v>
       </c>
       <c r="D399" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="E399" t="s">
         <v>66</v>
@@ -12401,7 +12560,7 @@
     </row>
     <row r="400" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B400" t="str">
         <f t="shared" si="25"/>
@@ -12412,7 +12571,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueorganization_secondary_location2</v>
       </c>
       <c r="D400" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="E400" t="s">
         <v>66</v>
@@ -12428,7 +12587,7 @@
     </row>
     <row r="401" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B401" t="str">
         <f t="shared" si="25"/>
@@ -12439,7 +12598,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuemy_locations</v>
       </c>
       <c r="D401" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E401" t="s">
         <v>69</v>
@@ -12455,7 +12614,7 @@
     </row>
     <row r="402" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B402" t="str">
         <f t="shared" si="25"/>
@@ -12479,7 +12638,7 @@
     </row>
     <row r="403" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B403" t="str">
         <f t="shared" si="25"/>
@@ -12490,7 +12649,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vuecreatedDatePicker</v>
       </c>
       <c r="D403" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="E403" t="s">
         <v>307</v>
@@ -12506,7 +12665,7 @@
     </row>
     <row r="404" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B404" t="str">
         <f t="shared" si="25"/>
@@ -12517,7 +12676,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteFilters.vueupdatedDatePicker</v>
       </c>
       <c r="D404" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E404" t="s">
         <v>307</v>
@@ -12533,7 +12692,7 @@
     </row>
     <row r="405" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B405" t="str">
         <f t="shared" si="25"/>
@@ -12560,7 +12719,7 @@
     </row>
     <row r="406" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B406" t="str">
         <f t="shared" si="25"/>
@@ -12585,9 +12744,9 @@
         <v>data-testid="testApplyFiltersButton"</v>
       </c>
     </row>
-    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B407" t="str">
         <f t="shared" si="25"/>
@@ -12598,7 +12757,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteImageSection.vueimageUploader</v>
       </c>
       <c r="D407" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="E407" t="s">
         <v>3</v>
@@ -12612,9 +12771,9 @@
         <v>data-testid="testImageUploaderFile"</v>
       </c>
     </row>
-    <row r="408" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B408" t="str">
         <f t="shared" si="25"/>
@@ -12625,7 +12784,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteImageSection.vueimageUploader</v>
       </c>
       <c r="D408" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="E408" t="s">
         <v>98</v>
@@ -12639,9 +12798,9 @@
         <v>data-testid="testImageUploaderModal"</v>
       </c>
     </row>
-    <row r="409" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B409" t="str">
         <f t="shared" si="25"/>
@@ -12649,1219 +12808,1319 @@
       </c>
       <c r="C409" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vue</v>
-      </c>
-      <c r="E409" t="str">
-        <f>IF(COUNTIF(C$2:C408,C409)&gt;0,"Button","")</f>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueintake_form</v>
+      </c>
+      <c r="D409" t="s">
+        <v>417</v>
+      </c>
+      <c r="E409" t="s">
+        <v>69</v>
       </c>
       <c r="F409" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testIntakeFormDiv</v>
       </c>
       <c r="G409" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIntakeFormDiv"</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B410" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C410" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E410" t="str">
-        <f>IF(COUNTIF(C$2:C409,C410)&gt;0,"Button","")</f>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuename</v>
+      </c>
+      <c r="D410" t="s">
+        <v>418</v>
+      </c>
+      <c r="E410" t="s">
+        <v>68</v>
       </c>
       <c r="F410" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testNameTextInput</v>
       </c>
       <c r="G410" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testNameTextInput"</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B411" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C411" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E411" t="str">
-        <f>IF(COUNTIF(C$2:C410,C411)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuephone1</v>
+      </c>
+      <c r="D411" t="s">
+        <v>419</v>
+      </c>
+      <c r="E411" t="s">
+        <v>68</v>
       </c>
       <c r="F411" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testPhone1TextInput</v>
       </c>
       <c r="G411" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testPhone1TextInput"</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B412" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C412" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E412" t="str">
-        <f>IF(COUNTIF(C$2:C411,C412)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuephone2</v>
+      </c>
+      <c r="D412" t="s">
+        <v>420</v>
+      </c>
+      <c r="E412" t="s">
+        <v>68</v>
       </c>
       <c r="F412" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testPhone2TextInput</v>
       </c>
       <c r="G412" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testPhone2TextInput"</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B413" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C413" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E413" t="str">
-        <f>IF(COUNTIF(C$2:C412,C413)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueadd_phone</v>
+      </c>
+      <c r="D413" t="s">
+        <v>421</v>
+      </c>
+      <c r="E413" t="s">
+        <v>91</v>
       </c>
       <c r="F413" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testAddPhoneLink</v>
       </c>
       <c r="G413" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testAddPhoneLink"</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B414" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C414" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E414" t="str">
-        <f>IF(COUNTIF(C$2:C413,C414)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueemail</v>
+      </c>
+      <c r="D414" t="s">
+        <v>422</v>
+      </c>
+      <c r="E414" t="s">
+        <v>68</v>
       </c>
       <c r="F414" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testEmailTextInput</v>
       </c>
       <c r="G414" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testEmailTextInput"</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B415" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C415" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E415" t="str">
-        <f>IF(COUNTIF(C$2:C414,C415)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueprimary_language</v>
+      </c>
+      <c r="D415" t="s">
+        <v>423</v>
+      </c>
+      <c r="E415" t="s">
+        <v>68</v>
       </c>
       <c r="F415" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testPrimaryLanguageTextInput</v>
       </c>
       <c r="G415" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testPrimaryLanguageTextInput"</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B416" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C416" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E416" t="str">
-        <f>IF(COUNTIF(C$2:C415,C416)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueauto_contact_frequency</v>
+      </c>
+      <c r="D416" t="s">
+        <v>424</v>
+      </c>
+      <c r="E416" t="s">
+        <v>87</v>
       </c>
       <c r="F416" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testAutoContactFrequencySelect</v>
       </c>
       <c r="G416" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testAutoContactFrequencySelect"</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B417" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C417" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E417" t="str">
-        <f>IF(COUNTIF(C$2:C416,C417)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuelocation_instructions</v>
+      </c>
+      <c r="D417" t="s">
+        <v>425</v>
+      </c>
+      <c r="E417" t="s">
+        <v>93</v>
       </c>
       <c r="F417" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testLocationInstructionsIcon</v>
       </c>
       <c r="G417" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testLocationInstructionsIcon"</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B418" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C418" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E418" t="str">
-        <f>IF(COUNTIF(C$2:C417,C418)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuelocation</v>
+      </c>
+      <c r="D418" t="s">
+        <v>310</v>
+      </c>
+      <c r="E418" t="s">
+        <v>93</v>
       </c>
       <c r="F418" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testLocationIcon</v>
       </c>
       <c r="G418" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testLocationIcon"</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B419" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C419" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E419" t="str">
-        <f>IF(COUNTIF(C$2:C418,C419)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueclear_location</v>
+      </c>
+      <c r="D419" t="s">
+        <v>426</v>
+      </c>
+      <c r="E419" t="s">
+        <v>93</v>
       </c>
       <c r="F419" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testClearLocationIcon</v>
       </c>
       <c r="G419" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testClearLocationIcon"</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B420" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C420" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E420" t="str">
-        <f>IF(COUNTIF(C$2:C419,C420)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuemanually_edit_address</v>
+      </c>
+      <c r="D420" t="s">
+        <v>427</v>
+      </c>
+      <c r="E420" t="s">
+        <v>93</v>
       </c>
       <c r="F420" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testManuallyEditAddressIcon</v>
       </c>
       <c r="G420" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testManuallyEditAddressIcon"</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B421" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C421" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E421" t="str">
-        <f>IF(COUNTIF(C$2:C420,C421)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuefull_address</v>
+      </c>
+      <c r="D421" t="s">
+        <v>428</v>
+      </c>
+      <c r="E421" t="s">
+        <v>68</v>
       </c>
       <c r="F421" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testFullAddressTextInput</v>
       </c>
       <c r="G421" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testFullAddressTextInput"</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B422" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C422" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E422" t="str">
-        <f>IF(COUNTIF(C$2:C421,C422)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueWorksiteSearchInput</v>
+      </c>
+      <c r="D422" t="s">
+        <v>429</v>
+      </c>
+      <c r="E422" t="s">
+        <v>307</v>
       </c>
       <c r="F422" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWorksiteSearchInputInput</v>
       </c>
       <c r="G422" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testWorksiteSearchInputInput"</v>
+      </c>
+    </row>
+    <row r="423" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B423" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C423" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E423" t="str">
-        <f>IF(COUNTIF(C$2:C422,C423)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuecity</v>
+      </c>
+      <c r="D423" t="s">
+        <v>430</v>
+      </c>
+      <c r="E423" t="s">
+        <v>68</v>
       </c>
       <c r="F423" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testCityTextInput</v>
       </c>
       <c r="G423" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCityTextInput"</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B424" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C424" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E424" t="str">
-        <f>IF(COUNTIF(C$2:C423,C424)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuecounty</v>
+      </c>
+      <c r="D424" t="s">
+        <v>431</v>
+      </c>
+      <c r="E424" t="s">
+        <v>68</v>
       </c>
       <c r="F424" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testCountyTextInput</v>
       </c>
       <c r="G424" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="425" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCountyTextInput"</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B425" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C425" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E425" t="str">
-        <f>IF(COUNTIF(C$2:C424,C425)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuestate</v>
+      </c>
+      <c r="D425" t="s">
+        <v>432</v>
+      </c>
+      <c r="E425" t="s">
+        <v>68</v>
       </c>
       <c r="F425" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testStateTextInput</v>
       </c>
       <c r="G425" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testStateTextInput"</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B426" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C426" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E426" t="str">
-        <f>IF(COUNTIF(C$2:C425,C426)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuewhat3words</v>
+      </c>
+      <c r="D426" t="s">
+        <v>433</v>
+      </c>
+      <c r="E426" t="s">
+        <v>68</v>
       </c>
       <c r="F426" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWhat3WordsTextInput</v>
       </c>
       <c r="G426" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testWhat3WordsTextInput"</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B427" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C427" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E427" t="str">
-        <f>IF(COUNTIF(C$2:C426,C427)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueuse_my_location</v>
+      </c>
+      <c r="D427" t="s">
+        <v>434</v>
+      </c>
+      <c r="E427" t="s">
+        <v>15</v>
       </c>
       <c r="F427" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testUseMyLocationButton</v>
       </c>
       <c r="G427" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testUseMyLocationButton"</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B428" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C428" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E428" t="str">
-        <f>IF(COUNTIF(C$2:C427,C428)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuetoggleSelectOnMap</v>
+      </c>
+      <c r="D428" t="s">
+        <v>435</v>
+      </c>
+      <c r="E428" t="s">
+        <v>15</v>
       </c>
       <c r="F428" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testToggleSelectOnMapButton</v>
       </c>
       <c r="G428" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testToggleSelectOnMapButton"</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B429" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C429" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E429" t="str">
-        <f>IF(COUNTIF(C$2:C428,C429)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuesaveNote</v>
+      </c>
+      <c r="D429" t="s">
+        <v>436</v>
+      </c>
+      <c r="E429" t="s">
+        <v>307</v>
       </c>
       <c r="F429" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testSaveNoteInput</v>
       </c>
       <c r="G429" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="430" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSaveNoteInput"</v>
+      </c>
+    </row>
+    <row r="430" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B430" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C430" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E430" t="str">
-        <f>IF(COUNTIF(C$2:C429,C430)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueaddress_problems</v>
+      </c>
+      <c r="D430" t="s">
+        <v>437</v>
+      </c>
+      <c r="E430" t="s">
+        <v>66</v>
       </c>
       <c r="F430" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testAddressProblemsCheckbox</v>
       </c>
       <c r="G430" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testAddressProblemsCheckbox"</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B431" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C431" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E431" t="str">
-        <f>IF(COUNTIF(C$2:C430,C431)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueisHighPriority</v>
+      </c>
+      <c r="D431" t="s">
+        <v>362</v>
+      </c>
+      <c r="E431" t="s">
+        <v>66</v>
       </c>
       <c r="F431" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testIsHighPriorityCheckbox</v>
       </c>
       <c r="G431" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIsHighPriorityCheckbox"</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B432" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C432" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E432" t="str">
-        <f>IF(COUNTIF(C$2:C431,C432)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuemember_of_my_org</v>
+      </c>
+      <c r="D432" t="s">
+        <v>361</v>
+      </c>
+      <c r="E432" t="s">
+        <v>66</v>
       </c>
       <c r="F432" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testMemberOfMyOrgCheckbox</v>
       </c>
       <c r="G432" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="433" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testMemberOfMyOrgCheckbox"</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B433" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C433" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vue:several_calculated</v>
+      </c>
+      <c r="D433" t="s">
+        <v>104</v>
       </c>
       <c r="E433" t="str">
         <f>IF(COUNTIF(C$2:C432,C433)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F433" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>test:SeveralCalculated</v>
       </c>
       <c r="G433" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="434" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="test:SeveralCalculated"</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B434" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C434" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E434" t="str">
-        <f>IF(COUNTIF(C$2:C433,C434)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueworksite.total_time</v>
+      </c>
+      <c r="D434" t="s">
+        <v>438</v>
+      </c>
+      <c r="E434" t="s">
+        <v>69</v>
       </c>
       <c r="F434" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWorksiteTotalTimeDiv</v>
       </c>
       <c r="G434" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testWorksiteTotalTimeDiv"</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B435" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C435" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E435" t="str">
-        <f>IF(COUNTIF(C$2:C434,C435)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vueworksiteImageSection</v>
+      </c>
+      <c r="D435" t="s">
+        <v>439</v>
+      </c>
+      <c r="E435" t="s">
+        <v>69</v>
       </c>
       <c r="F435" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWorksiteImageSectionDiv</v>
       </c>
       <c r="G435" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="436" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testWorksiteImageSectionDiv"</v>
+      </c>
+    </row>
+    <row r="436" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B436" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C436" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E436" t="str">
-        <f>IF(COUNTIF(C$2:C435,C436)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuecloseWorksite</v>
+      </c>
+      <c r="D436" t="s">
+        <v>359</v>
+      </c>
+      <c r="E436" t="s">
+        <v>15</v>
       </c>
       <c r="F436" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testCloseWorksiteButton</v>
       </c>
       <c r="G436" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="437" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCloseWorksiteButton"</v>
+      </c>
+    </row>
+    <row r="437" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B437" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C437" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E437" t="str">
-        <f>IF(COUNTIF(C$2:C436,C437)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuesave</v>
+      </c>
+      <c r="D437" t="s">
+        <v>169</v>
+      </c>
+      <c r="E437" t="s">
+        <v>15</v>
       </c>
       <c r="F437" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testSaveButton</v>
       </c>
       <c r="G437" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="438" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSaveButton"</v>
+      </c>
+    </row>
+    <row r="438" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B438" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C438" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E438" t="str">
-        <f>IF(COUNTIF(C$2:C437,C438)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuesave_claim</v>
+      </c>
+      <c r="D438" t="s">
+        <v>440</v>
+      </c>
+      <c r="E438" t="s">
+        <v>15</v>
       </c>
       <c r="F438" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testSaveClaimButton</v>
       </c>
       <c r="G438" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="439" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSaveClaimButton"</v>
+      </c>
+    </row>
+    <row r="439" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>330</v>
+        <v>416</v>
       </c>
       <c r="B439" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteForm.vue</v>
       </c>
       <c r="C439" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E439" t="str">
-        <f>IF(COUNTIF(C$2:C438,C439)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteForm.vuepostal_code</v>
+      </c>
+      <c r="D439" t="s">
+        <v>441</v>
+      </c>
+      <c r="E439" t="s">
+        <v>68</v>
       </c>
       <c r="F439" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testPostalCodeTextInput</v>
       </c>
       <c r="G439" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="440" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testPostalCodeTextInput"</v>
+      </c>
+    </row>
+    <row r="440" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>330</v>
+        <v>442</v>
       </c>
       <c r="B440" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteNotes.vue</v>
       </c>
       <c r="C440" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E440" t="str">
-        <f>IF(COUNTIF(C$2:C439,C440)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes.vueworksite_notes</v>
+      </c>
+      <c r="D440" t="s">
+        <v>443</v>
+      </c>
+      <c r="E440" t="s">
+        <v>69</v>
       </c>
       <c r="F440" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWorksiteNotesDiv</v>
       </c>
       <c r="G440" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="441" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testWorksiteNotesDiv"</v>
+      </c>
+    </row>
+    <row r="441" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>330</v>
+        <v>442</v>
       </c>
       <c r="B441" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteNotes.vue</v>
       </c>
       <c r="C441" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E441" t="str">
-        <f>IF(COUNTIF(C$2:C440,C441)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes.vueshowAllNotes</v>
+      </c>
+      <c r="D441" t="s">
+        <v>444</v>
+      </c>
+      <c r="E441" t="s">
+        <v>15</v>
       </c>
       <c r="F441" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testShowAllNotesButton</v>
       </c>
       <c r="G441" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="442" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testShowAllNotesButton"</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>330</v>
+        <v>442</v>
       </c>
       <c r="B442" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteNotes.vue</v>
       </c>
       <c r="C442" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E442" t="str">
-        <f>IF(COUNTIF(C$2:C441,C442)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes.vueshowNotes</v>
+      </c>
+      <c r="D442" t="s">
+        <v>445</v>
+      </c>
+      <c r="E442" t="s">
+        <v>69</v>
       </c>
       <c r="F442" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testShowNotesDiv</v>
       </c>
       <c r="G442" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="443" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testShowNotesDiv"</v>
+      </c>
+    </row>
+    <row r="443" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>330</v>
+        <v>442</v>
       </c>
       <c r="B443" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteNotes.vue</v>
       </c>
       <c r="C443" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E443" t="str">
-        <f>IF(COUNTIF(C$2:C442,C443)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes.vueadd_note</v>
+      </c>
+      <c r="D443" t="s">
+        <v>446</v>
+      </c>
+      <c r="E443" t="s">
+        <v>15</v>
       </c>
       <c r="F443" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testAddNoteButton</v>
       </c>
       <c r="G443" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="444" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testAddNoteButton"</v>
+      </c>
+    </row>
+    <row r="444" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>330</v>
+        <v>442</v>
       </c>
       <c r="B444" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteNotes.vue</v>
       </c>
       <c r="C444" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E444" t="str">
-        <f>IF(COUNTIF(C$2:C443,C444)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes.vuesticky_note</v>
+      </c>
+      <c r="D444" t="s">
+        <v>447</v>
+      </c>
+      <c r="E444" t="s">
+        <v>93</v>
       </c>
       <c r="F444" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testStickyNoteIcon</v>
       </c>
       <c r="G444" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="445" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testStickyNoteIcon"</v>
+      </c>
+    </row>
+    <row r="445" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>330</v>
+        <v>442</v>
       </c>
       <c r="B445" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteNotes.vue</v>
       </c>
       <c r="C445" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E445" t="str">
-        <f>IF(COUNTIF(C$2:C444,C445)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes.vuecurrentNote</v>
+      </c>
+      <c r="D445" t="s">
+        <v>448</v>
+      </c>
+      <c r="E445" t="s">
+        <v>67</v>
       </c>
       <c r="F445" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testCurrentNoteTextarea</v>
       </c>
       <c r="G445" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="446" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCurrentNoteTextarea"</v>
+      </c>
+    </row>
+    <row r="446" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>330</v>
+        <v>442</v>
       </c>
       <c r="B446" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteNotes.vue</v>
       </c>
       <c r="C446" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E446" t="str">
-        <f>IF(COUNTIF(C$2:C445,C446)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes.vuecancelNote</v>
+      </c>
+      <c r="D446" t="s">
+        <v>449</v>
+      </c>
+      <c r="E446" t="s">
+        <v>15</v>
       </c>
       <c r="F446" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testCancelNoteButton</v>
       </c>
       <c r="G446" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="447" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCancelNoteButton"</v>
+      </c>
+    </row>
+    <row r="447" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>330</v>
+        <v>442</v>
       </c>
       <c r="B447" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteNotes.vue</v>
       </c>
       <c r="C447" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E447" t="str">
-        <f>IF(COUNTIF(C$2:C446,C447)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes.vuesaveNote</v>
+      </c>
+      <c r="D447" t="s">
+        <v>436</v>
+      </c>
+      <c r="E447" t="s">
+        <v>15</v>
       </c>
       <c r="F447" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testSaveNoteButton</v>
       </c>
       <c r="G447" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="448" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSaveNoteButton"</v>
+      </c>
+    </row>
+    <row r="448" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>330</v>
+        <v>450</v>
       </c>
       <c r="B448" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteReportSection.vue</v>
       </c>
       <c r="C448" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E448" t="str">
-        <f>IF(COUNTIF(C$2:C447,C448)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteReportSection.vuevolunteersToAdd</v>
+      </c>
+      <c r="D448" t="s">
+        <v>451</v>
+      </c>
+      <c r="E448" t="s">
+        <v>68</v>
       </c>
       <c r="F448" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testVolunteersToAddTextInput</v>
       </c>
       <c r="G448" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="449" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testVolunteersToAddTextInput"</v>
+      </c>
+    </row>
+    <row r="449" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>330</v>
+        <v>450</v>
       </c>
       <c r="B449" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteReportSection.vue</v>
       </c>
       <c r="C449" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E449" t="str">
-        <f>IF(COUNTIF(C$2:C448,C449)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteReportSection.vuehoursPerVolunteer</v>
+      </c>
+      <c r="D449" t="s">
+        <v>452</v>
+      </c>
+      <c r="E449" t="s">
+        <v>68</v>
       </c>
       <c r="F449" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testHoursPerVolunteerTextInput</v>
       </c>
       <c r="G449" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="450" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testHoursPerVolunteerTextInput"</v>
+      </c>
+    </row>
+    <row r="450" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>330</v>
+        <v>450</v>
       </c>
       <c r="B450" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteReportSection.vue</v>
       </c>
       <c r="C450" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E450" t="str">
-        <f>IF(COUNTIF(C$2:C449,C450)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteReportSection.vueaddTime</v>
+      </c>
+      <c r="D450" t="s">
+        <v>453</v>
+      </c>
+      <c r="E450" t="s">
+        <v>15</v>
       </c>
       <c r="F450" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testAddTimeButton</v>
       </c>
       <c r="G450" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="451" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testAddTimeButton"</v>
+      </c>
+    </row>
+    <row r="451" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>330</v>
+        <v>450</v>
       </c>
       <c r="B451" t="str">
         <f t="shared" si="25"/>
-        <v/>
+        <v>WorksiteReportSection.vue</v>
       </c>
       <c r="C451" t="str">
         <f t="shared" si="26"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E451" t="str">
-        <f>IF(COUNTIF(C$2:C450,C451)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteReportSection.vuetotal_volunteers</v>
+      </c>
+      <c r="D451" t="s">
+        <v>454</v>
+      </c>
+      <c r="E451" t="s">
+        <v>69</v>
       </c>
       <c r="F451" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testTotalVolunteersDiv</v>
       </c>
       <c r="G451" t="str">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-    </row>
-    <row r="452" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testTotalVolunteersDiv"</v>
+      </c>
+    </row>
+    <row r="452" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>330</v>
+        <v>450</v>
       </c>
       <c r="B452" t="str">
         <f t="shared" ref="B452:B501" si="29">IF(A452="","",MID(A452,FIND("@",SUBSTITUTE(A452,"\","@",LEN(A452)-LEN(SUBSTITUTE(A452,"\",""))))+1,LEN(A452)))</f>
-        <v/>
+        <v>WorksiteReportSection.vue</v>
       </c>
       <c r="C452" t="str">
         <f t="shared" ref="C452:C501" si="30">A452&amp;D452</f>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E452" t="str">
-        <f>IF(COUNTIF(C$2:C451,C452)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteReportSection.vuecurrentTimeEdit</v>
+      </c>
+      <c r="D452" t="s">
+        <v>455</v>
+      </c>
+      <c r="E452" t="s">
+        <v>93</v>
       </c>
       <c r="F452" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testCurrentTimeEditIcon</v>
       </c>
       <c r="G452" t="str">
         <f t="shared" ref="G452:G501" si="31">IF(D452="","","data-testid="""&amp;F452&amp;"""")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="453" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCurrentTimeEditIcon"</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>330</v>
+        <v>450</v>
       </c>
       <c r="B453" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>WorksiteReportSection.vue</v>
       </c>
       <c r="C453" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E453" t="str">
-        <f>IF(COUNTIF(C$2:C452,C453)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteReportSection.vuecurrentTimeSave</v>
+      </c>
+      <c r="D453" t="s">
+        <v>456</v>
+      </c>
+      <c r="E453" t="s">
+        <v>93</v>
       </c>
       <c r="F453" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testCurrentTimeSaveIcon</v>
       </c>
       <c r="G453" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="454" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCurrentTimeSaveIcon"</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>330</v>
+        <v>457</v>
       </c>
       <c r="B454" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>WorksiteSearchInput.vue</v>
       </c>
       <c r="C454" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E454" t="str">
-        <f>IF(COUNTIF(C$2:C453,C454)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteSearchInput.vueWorksiteSearchInput</v>
+      </c>
+      <c r="D454" t="s">
+        <v>429</v>
+      </c>
+      <c r="E454" t="s">
+        <v>216</v>
       </c>
       <c r="F454" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWorksiteSearchInputSearch</v>
       </c>
       <c r="G454" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="455" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testWorksiteSearchInputSearch"</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>330</v>
+        <v>457</v>
       </c>
       <c r="B455" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>WorksiteSearchInput.vue</v>
       </c>
       <c r="C455" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E455" t="str">
-        <f>IF(COUNTIF(C$2:C454,C455)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteSearchInput.vueworsiteSearchResults</v>
+      </c>
+      <c r="D455" t="s">
+        <v>458</v>
+      </c>
+      <c r="E455" t="s">
+        <v>69</v>
       </c>
       <c r="F455" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWorsiteSearchResultsDiv</v>
       </c>
       <c r="G455" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="456" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testWorsiteSearchResultsDiv"</v>
+      </c>
+    </row>
+    <row r="456" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>330</v>
+        <v>459</v>
       </c>
       <c r="B456" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>WorksiteTable.vue</v>
       </c>
       <c r="C456" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E456" t="str">
-        <f>IF(COUNTIF(C$2:C455,C456)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteTable.vueworksiteTable</v>
+      </c>
+      <c r="D456" t="s">
+        <v>460</v>
+      </c>
+      <c r="E456" t="s">
+        <v>69</v>
       </c>
       <c r="F456" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWorksiteTableDiv</v>
       </c>
       <c r="G456" t="str">
         <f t="shared" si="31"/>
-        <v/>
+        <v>data-testid="testWorksiteTableDiv"</v>
       </c>
     </row>
     <row r="457" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>330</v>
+        <v>461</v>
       </c>
       <c r="B457" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>WorksiteView.vue</v>
       </c>
       <c r="C457" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteView.vue:several_calculated</v>
+      </c>
+      <c r="D457" t="s">
+        <v>104</v>
       </c>
       <c r="E457" t="str">
         <f>IF(COUNTIF(C$2:C456,C457)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F457" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>test:SeveralCalculated</v>
       </c>
       <c r="G457" t="str">
         <f t="shared" si="31"/>
-        <v/>
+        <v>data-testid="test:SeveralCalculated"</v>
       </c>
     </row>
     <row r="458" spans="1:7" x14ac:dyDescent="0.25">
@@ -13874,19 +14133,21 @@
       </c>
       <c r="C458" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E458" t="str">
-        <f>IF(COUNTIF(C$2:C457,C458)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\worksiteFormContent</v>
+      </c>
+      <c r="D458" t="s">
+        <v>462</v>
+      </c>
+      <c r="E458" t="s">
+        <v>69</v>
       </c>
       <c r="F458" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWorksiteFormContentDiv</v>
       </c>
       <c r="G458" t="str">
         <f t="shared" si="31"/>
-        <v/>
+        <v>data-testid="testWorksiteFormContentDiv"</v>
       </c>
     </row>
     <row r="459" spans="1:7" x14ac:dyDescent="0.25">
@@ -13899,19 +14160,21 @@
       </c>
       <c r="C459" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E459" t="str">
-        <f>IF(COUNTIF(C$2:C458,C459)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\WorksiteNotes</v>
+      </c>
+      <c r="D459" t="s">
+        <v>463</v>
+      </c>
+      <c r="E459" t="s">
+        <v>92</v>
       </c>
       <c r="F459" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testWorksiteNotesContent</v>
       </c>
       <c r="G459" t="str">
         <f t="shared" si="31"/>
-        <v/>
+        <v>data-testid="testWorksiteNotesContent"</v>
       </c>
     </row>
     <row r="460" spans="1:7" x14ac:dyDescent="0.25">
@@ -13924,19 +14187,21 @@
       </c>
       <c r="C460" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E460" t="str">
-        <f>IF(COUNTIF(C$2:C459,C460)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\name</v>
+      </c>
+      <c r="D460" t="s">
+        <v>418</v>
+      </c>
+      <c r="E460" t="s">
+        <v>92</v>
       </c>
       <c r="F460" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testNameContent</v>
       </c>
       <c r="G460" t="str">
         <f t="shared" si="31"/>
-        <v/>
+        <v>data-testid="testNameContent"</v>
       </c>
     </row>
     <row r="461" spans="1:7" x14ac:dyDescent="0.25">
@@ -13949,19 +14214,21 @@
       </c>
       <c r="C461" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E461" t="str">
-        <f>IF(COUNTIF(C$2:C460,C461)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\phone</v>
+      </c>
+      <c r="D461" t="s">
+        <v>464</v>
+      </c>
+      <c r="E461" t="s">
+        <v>92</v>
       </c>
       <c r="F461" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testPhoneContent</v>
       </c>
       <c r="G461" t="str">
         <f t="shared" si="31"/>
-        <v/>
+        <v>data-testid="testPhoneContent"</v>
       </c>
     </row>
     <row r="462" spans="1:7" x14ac:dyDescent="0.25">
@@ -13974,19 +14241,21 @@
       </c>
       <c r="C462" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E462" t="str">
-        <f>IF(COUNTIF(C$2:C461,C462)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\call_number</v>
+      </c>
+      <c r="D462" t="s">
+        <v>465</v>
+      </c>
+      <c r="E462" t="s">
+        <v>15</v>
       </c>
       <c r="F462" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testCallNumberButton</v>
       </c>
       <c r="G462" t="str">
         <f t="shared" si="31"/>
-        <v/>
+        <v>data-testid="testCallNumberButton"</v>
       </c>
     </row>
     <row r="463" spans="1:7" x14ac:dyDescent="0.25">
@@ -13999,19 +14268,21 @@
       </c>
       <c r="C463" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E463" t="str">
-        <f>IF(COUNTIF(C$2:C462,C463)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\address</v>
+      </c>
+      <c r="D463" t="s">
+        <v>466</v>
+      </c>
+      <c r="E463" t="s">
+        <v>92</v>
       </c>
       <c r="F463" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testAddressContent</v>
       </c>
       <c r="G463" t="str">
         <f t="shared" si="31"/>
-        <v/>
+        <v>data-testid="testAddressContent"</v>
       </c>
     </row>
     <row r="464" spans="1:7" x14ac:dyDescent="0.25">
@@ -14024,19 +14295,21 @@
       </c>
       <c r="C464" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\</v>
-      </c>
-      <c r="E464" t="str">
-        <f>IF(COUNTIF(C$2:C463,C464)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\work\claim_all</v>
+      </c>
+      <c r="D464" t="s">
+        <v>467</v>
+      </c>
+      <c r="E464" t="s">
+        <v>15</v>
       </c>
       <c r="F464" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>testClaimAllButton</v>
       </c>
       <c r="G464" t="str">
         <f t="shared" si="31"/>
-        <v/>
+        <v>data-testid="testClaimAllButton"</v>
       </c>
     </row>
     <row r="465" spans="1:7" x14ac:dyDescent="0.25">
@@ -14053,7 +14326,7 @@
       </c>
       <c r="E465" t="str">
         <f>IF(COUNTIF(C$2:C464,C465)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F465" t="str">
         <f t="shared" ref="F465:F501" si="32">IF(D465="","","test"&amp;IF(ISNUMBER(SEARCH(".",D465)),UPPER(LEFT(D465,1))&amp;RIGHT(LEFT(D465,SEARCH(".",D465)-1),LEN(LEFT(D465,SEARCH(".",D465)-1))-1)&amp;SUBSTITUTE(PROPER(RIGHT(D465,LEN(D465)-SEARCH(".",D465))),"_",""),IF(EXACT(LOWER(D465),D465),TRIM(SUBSTITUTE(PROPER(D465),"_","")),UPPER(LEFT(D465,1))&amp;RIGHT(D465,LEN(D465)-1)))&amp;E465)</f>

</xml_diff>

<commit_message>
Components files A-S, data-testids
(cherry picked from commit c325ace040811b7604536ae96495e10daa3a333b)
</commit_message>
<xml_diff>
--- a/test/e2e/List of data-testids.xlsx
+++ b/test/e2e/List of data-testids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\test\e2e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1BFC3F-227D-4F2B-8FFA-6D4C4C2B1EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0735F8-D499-4CD1-A448-BA42F1FA0134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4245" yWindow="975" windowWidth="18810" windowHeight="12585" xr2:uid="{51F30F27-9EA9-4B4D-86A3-E32FA30758F4}"/>
+    <workbookView xWindow="60" yWindow="840" windowWidth="14580" windowHeight="12585" xr2:uid="{51F30F27-9EA9-4B4D-86A3-E32FA30758F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="553">
   <si>
     <t>Output</t>
   </si>
@@ -1493,6 +1493,201 @@
   </si>
   <si>
     <t>table</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Badge.vue</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Avatar.vue</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>badge</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\BugReport.vue</t>
+  </si>
+  <si>
+    <t>BugTitle</t>
+  </si>
+  <si>
+    <t>bug.description</t>
+  </si>
+  <si>
+    <t>bug.upload</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Capability.vue</t>
+  </si>
+  <si>
+    <t>capabilityTable</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\CapabilityItem.vue</t>
+  </si>
+  <si>
+    <t>capability</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\CapabilityGrid.vue</t>
+  </si>
+  <si>
+    <t>capabilityGrid</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\EventTimeline.vue</t>
+  </si>
+  <si>
+    <t>UserDetails</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\ImageModal.vue</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\IncidentContact.vue</t>
+  </si>
+  <si>
+    <t>survivorContact</t>
+  </si>
+  <si>
+    <t>spinnerLoading</t>
+  </si>
+  <si>
+    <t>IncidentPhone</t>
+  </si>
+  <si>
+    <t>NoPhone</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\ItemEditor.vue</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\LoginForm.vue</t>
+  </si>
+  <si>
+    <t>login_text</t>
+  </si>
+  <si>
+    <t>signin_text</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>request_password_reset</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>request_access</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Modal.vue</t>
+  </si>
+  <si>
+    <t>modalCancel</t>
+  </si>
+  <si>
+    <t>modalCancel2</t>
+  </si>
+  <si>
+    <t>modalOk</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\PdfViewer.vue</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\OrganizationSearchInput.vue</t>
+  </si>
+  <si>
+    <t>organization_name</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RecurringSchedule.vue</t>
+  </si>
+  <si>
+    <t>schedule_frequency</t>
+  </si>
+  <si>
+    <t>dailyOption</t>
+  </si>
+  <si>
+    <t>dayInterval</t>
+  </si>
+  <si>
+    <t>every_weekday_interval</t>
+  </si>
+  <si>
+    <t>calendar</t>
+  </si>
+  <si>
+    <t>endDatePicker</t>
+  </si>
+  <si>
+    <t>add_schedule</t>
+  </si>
+  <si>
+    <t>requestIncident</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RequestRedeploy.vue</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\SimpleMap.vue</t>
+  </si>
+  <si>
+    <t>zoom_out</t>
+  </si>
+  <si>
+    <t>zoom_to_make_interactive</t>
+  </si>
+  <si>
+    <t>zoom_to_incident</t>
+  </si>
+  <si>
+    <t>showLegend</t>
+  </si>
+  <si>
+    <t>zoom_in</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\DisasterIcon.vue</t>
+  </si>
+  <si>
+    <t>randomEasterEgg</t>
+  </si>
+  <si>
+    <t>incidentImage</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Slider.vue</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Tag.vue</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Table.vue</t>
+  </si>
+  <si>
+    <t>setAllChecked</t>
+  </si>
+  <si>
+    <t>no_items_found</t>
+  </si>
+  <si>
+    <t>pagination.pageSize</t>
+  </si>
+  <si>
+    <t>pagination.prev</t>
+  </si>
+  <si>
+    <t>pagination.next</t>
   </si>
 </sst>
 </file>
@@ -1848,7 +2043,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F495" sqref="F495"/>
+      <selection pane="bottomLeft" activeCell="B541" sqref="B541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14940,7 +15135,7 @@
         <v>data-testid="testRequestButton"</v>
       </c>
     </row>
-    <row r="486" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>485</v>
       </c>
@@ -14967,17 +15162,17 @@
         <v>data-testid="testTableSearchTextInput"</v>
       </c>
     </row>
-    <row r="487" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B487" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>AjaxTable.vue</v>
       </c>
       <c r="C487" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\table</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\AjaxTable.vuetable</v>
       </c>
       <c r="D487" t="s">
         <v>487</v>
@@ -14994,1404 +15189,1517 @@
         <v>data-testid="testTableContent"</v>
       </c>
     </row>
-    <row r="488" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="B488" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>Avatar.vue</v>
       </c>
       <c r="C488" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E488" t="str">
-        <f>IF(COUNTIF(C$2:C487,C488)&gt;0,"Button","")</f>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Avatar.vueavatar</v>
+      </c>
+      <c r="D488" t="s">
+        <v>490</v>
+      </c>
+      <c r="E488" t="s">
+        <v>93</v>
       </c>
       <c r="F488" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testAvatarIcon</v>
       </c>
       <c r="G488" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="489" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testAvatarIcon"</v>
+      </c>
+    </row>
+    <row r="489" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B489" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>Badge.vue</v>
       </c>
       <c r="C489" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E489" t="str">
-        <f>IF(COUNTIF(C$2:C488,C489)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Badge.vuebadge</v>
+      </c>
+      <c r="D489" t="s">
+        <v>491</v>
+      </c>
+      <c r="E489" t="s">
+        <v>69</v>
       </c>
       <c r="F489" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testBadgeDiv</v>
       </c>
       <c r="G489" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="490" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testBadgeDiv"</v>
+      </c>
+    </row>
+    <row r="490" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="B490" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>BugReport.vue</v>
       </c>
       <c r="C490" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E490" t="str">
-        <f>IF(COUNTIF(C$2:C489,C490)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\BugReport.vueBugTitle</v>
+      </c>
+      <c r="D490" t="s">
+        <v>493</v>
+      </c>
+      <c r="E490" t="s">
+        <v>68</v>
       </c>
       <c r="F490" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testBugTitleTextInput</v>
       </c>
       <c r="G490" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="491" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testBugTitleTextInput"</v>
+      </c>
+    </row>
+    <row r="491" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="B491" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>BugReport.vue</v>
       </c>
       <c r="C491" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E491" t="str">
-        <f>IF(COUNTIF(C$2:C490,C491)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\BugReport.vuebug.description</v>
+      </c>
+      <c r="D491" t="s">
+        <v>494</v>
+      </c>
+      <c r="E491" t="s">
+        <v>68</v>
       </c>
       <c r="F491" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testBugDescriptionTextInput</v>
       </c>
       <c r="G491" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="492" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testBugDescriptionTextInput"</v>
+      </c>
+    </row>
+    <row r="492" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="B492" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>BugReport.vue</v>
       </c>
       <c r="C492" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E492" t="str">
-        <f>IF(COUNTIF(C$2:C491,C492)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\BugReport.vuebug.upload</v>
+      </c>
+      <c r="D492" t="s">
+        <v>495</v>
+      </c>
+      <c r="E492" t="s">
+        <v>3</v>
       </c>
       <c r="F492" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testBugUploadFile</v>
       </c>
       <c r="G492" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="493" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testBugUploadFile"</v>
+      </c>
+    </row>
+    <row r="493" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="B493" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>BugReport.vue</v>
       </c>
       <c r="C493" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E493" t="str">
-        <f>IF(COUNTIF(C$2:C492,C493)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\BugReport.vuesubmit</v>
+      </c>
+      <c r="D493" t="s">
+        <v>212</v>
+      </c>
+      <c r="E493" t="s">
+        <v>15</v>
       </c>
       <c r="F493" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testSubmitButton</v>
       </c>
       <c r="G493" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="494" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSubmitButton"</v>
+      </c>
+    </row>
+    <row r="494" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="B494" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>Capability.vue</v>
       </c>
       <c r="C494" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E494" t="str">
-        <f>IF(COUNTIF(C$2:C493,C494)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Capability.vuecapabilityTable</v>
+      </c>
+      <c r="D494" t="s">
+        <v>497</v>
+      </c>
+      <c r="E494" t="s">
+        <v>69</v>
       </c>
       <c r="F494" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testCapabilityTableDiv</v>
       </c>
       <c r="G494" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="495" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCapabilityTableDiv"</v>
+      </c>
+    </row>
+    <row r="495" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="B495" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>Capability.vue</v>
       </c>
       <c r="C495" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Capability.vue:several_calculated</v>
+      </c>
+      <c r="D495" t="s">
+        <v>104</v>
       </c>
       <c r="E495" t="str">
         <f>IF(COUNTIF(C$2:C494,C495)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F495" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>test:SeveralCalculated</v>
       </c>
       <c r="G495" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="496" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="test:SeveralCalculated"</v>
+      </c>
+    </row>
+    <row r="496" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
       <c r="B496" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>CapabilityItem.vue</v>
       </c>
       <c r="C496" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E496" t="str">
-        <f>IF(COUNTIF(C$2:C495,C496)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\CapabilityItem.vuecapability</v>
+      </c>
+      <c r="D496" t="s">
+        <v>499</v>
+      </c>
+      <c r="E496" t="s">
+        <v>99</v>
       </c>
       <c r="F496" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testCapabilityTooltip</v>
       </c>
       <c r="G496" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="497" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCapabilityTooltip"</v>
+      </c>
+    </row>
+    <row r="497" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
       <c r="B497" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>CapabilityItem.vue</v>
       </c>
       <c r="C497" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\CapabilityItem.vue:several_calculated</v>
+      </c>
+      <c r="D497" t="s">
+        <v>104</v>
       </c>
       <c r="E497" t="str">
         <f>IF(COUNTIF(C$2:C496,C497)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F497" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>test:SeveralCalculated</v>
       </c>
       <c r="G497" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="498" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="test:SeveralCalculated"</v>
+      </c>
+    </row>
+    <row r="498" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>484</v>
+        <v>500</v>
       </c>
       <c r="B498" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>CapabilityGrid.vue</v>
       </c>
       <c r="C498" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E498" t="str">
-        <f>IF(COUNTIF(C$2:C497,C498)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\CapabilityGrid.vuecapabilityGrid</v>
+      </c>
+      <c r="D498" t="s">
+        <v>501</v>
+      </c>
+      <c r="E498" t="s">
+        <v>69</v>
       </c>
       <c r="F498" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testCapabilityGridDiv</v>
       </c>
       <c r="G498" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="499" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCapabilityGridDiv"</v>
+      </c>
+    </row>
+    <row r="499" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>484</v>
+        <v>500</v>
       </c>
       <c r="B499" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>CapabilityGrid.vue</v>
       </c>
       <c r="C499" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\CapabilityGrid.vue:several_calculated</v>
+      </c>
+      <c r="D499" t="s">
+        <v>104</v>
       </c>
       <c r="E499" t="str">
         <f>IF(COUNTIF(C$2:C498,C499)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F499" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>test:SeveralCalculated</v>
       </c>
       <c r="G499" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="500" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="test:SeveralCalculated"</v>
+      </c>
+    </row>
+    <row r="500" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>484</v>
+        <v>502</v>
       </c>
       <c r="B500" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>EventTimeline.vue</v>
       </c>
       <c r="C500" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E500" t="str">
-        <f>IF(COUNTIF(C$2:C499,C500)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\EventTimeline.vueUserDetails</v>
+      </c>
+      <c r="D500" t="s">
+        <v>503</v>
+      </c>
+      <c r="E500" t="s">
+        <v>99</v>
       </c>
       <c r="F500" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testUserDetailsTooltip</v>
       </c>
       <c r="G500" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="501" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testUserDetailsTooltip"</v>
+      </c>
+    </row>
+    <row r="501" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>484</v>
+        <v>504</v>
       </c>
       <c r="B501" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>ImageModal.vue</v>
       </c>
       <c r="C501" t="str">
         <f t="shared" si="30"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E501" t="str">
-        <f>IF(COUNTIF(C$2:C500,C501)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\ImageModal.vuedelete</v>
+      </c>
+      <c r="D501" t="s">
+        <v>505</v>
+      </c>
+      <c r="E501" t="s">
+        <v>15</v>
       </c>
       <c r="F501" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>testDeleteButton</v>
       </c>
       <c r="G501" t="str">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-    </row>
-    <row r="502" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testDeleteButton"</v>
+      </c>
+    </row>
+    <row r="502" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>484</v>
+        <v>506</v>
       </c>
       <c r="B502" t="str">
         <f t="shared" ref="B502:B565" si="33">IF(A502="","",MID(A502,FIND("@",SUBSTITUTE(A502,"\","@",LEN(A502)-LEN(SUBSTITUTE(A502,"\",""))))+1,LEN(A502)))</f>
-        <v/>
+        <v>IncidentContact.vue</v>
       </c>
       <c r="C502" t="str">
         <f t="shared" ref="C502:C565" si="34">A502&amp;D502</f>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E502" t="str">
-        <f>IF(COUNTIF(C$2:C501,C502)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\IncidentContact.vuesurvivorContact</v>
+      </c>
+      <c r="D502" t="s">
+        <v>507</v>
+      </c>
+      <c r="E502" t="s">
+        <v>69</v>
       </c>
       <c r="F502" t="str">
         <f t="shared" ref="F502:F565" si="35">IF(D502="","","test"&amp;IF(ISNUMBER(SEARCH(".",D502)),UPPER(LEFT(D502,1))&amp;RIGHT(LEFT(D502,SEARCH(".",D502)-1),LEN(LEFT(D502,SEARCH(".",D502)-1))-1)&amp;SUBSTITUTE(PROPER(RIGHT(D502,LEN(D502)-SEARCH(".",D502))),"_",""),IF(EXACT(LOWER(D502),D502),TRIM(SUBSTITUTE(PROPER(D502),"_","")),UPPER(LEFT(D502,1))&amp;RIGHT(D502,LEN(D502)-1)))&amp;E502)</f>
-        <v/>
+        <v>testSurvivorContactDiv</v>
       </c>
       <c r="G502" t="str">
         <f t="shared" ref="G502:G565" si="36">IF(D502="","","data-testid="""&amp;F502&amp;"""")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="503" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSurvivorContactDiv"</v>
+      </c>
+    </row>
+    <row r="503" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>484</v>
+        <v>506</v>
       </c>
       <c r="B503" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>IncidentContact.vue</v>
       </c>
       <c r="C503" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E503" t="str">
-        <f>IF(COUNTIF(C$2:C502,C503)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\IncidentContact.vuespinnerLoading</v>
+      </c>
+      <c r="D503" t="s">
+        <v>508</v>
+      </c>
+      <c r="E503" t="s">
+        <v>93</v>
       </c>
       <c r="F503" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testSpinnerLoadingIcon</v>
       </c>
       <c r="G503" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="504" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSpinnerLoadingIcon"</v>
+      </c>
+    </row>
+    <row r="504" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>484</v>
+        <v>506</v>
       </c>
       <c r="B504" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>IncidentContact.vue</v>
       </c>
       <c r="C504" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E504" t="str">
-        <f>IF(COUNTIF(C$2:C503,C504)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\IncidentContact.vueIncidentPhone</v>
+      </c>
+      <c r="D504" t="s">
+        <v>509</v>
+      </c>
+      <c r="E504" t="s">
+        <v>69</v>
       </c>
       <c r="F504" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testIncidentPhoneDiv</v>
       </c>
       <c r="G504" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="505" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testIncidentPhoneDiv"</v>
+      </c>
+    </row>
+    <row r="505" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>484</v>
+        <v>506</v>
       </c>
       <c r="B505" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>IncidentContact.vue</v>
       </c>
       <c r="C505" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E505" t="str">
-        <f>IF(COUNTIF(C$2:C504,C505)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\IncidentContact.vueNoPhone</v>
+      </c>
+      <c r="D505" t="s">
+        <v>510</v>
+      </c>
+      <c r="E505" t="s">
+        <v>69</v>
       </c>
       <c r="F505" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testNoPhoneDiv</v>
       </c>
       <c r="G505" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="506" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testNoPhoneDiv"</v>
+      </c>
+    </row>
+    <row r="506" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>484</v>
+        <v>511</v>
       </c>
       <c r="B506" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>ItemEditor.vue</v>
       </c>
       <c r="C506" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E506" t="str">
-        <f>IF(COUNTIF(C$2:C505,C506)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\ItemEditor.vueedit</v>
+      </c>
+      <c r="D506" t="s">
+        <v>371</v>
+      </c>
+      <c r="E506" t="s">
+        <v>15</v>
       </c>
       <c r="F506" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testEditButton</v>
       </c>
       <c r="G506" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="507" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testEditButton"</v>
+      </c>
+    </row>
+    <row r="507" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>484</v>
+        <v>511</v>
       </c>
       <c r="B507" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>ItemEditor.vue</v>
       </c>
       <c r="C507" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E507" t="str">
-        <f>IF(COUNTIF(C$2:C506,C507)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\ItemEditor.vuedelete</v>
+      </c>
+      <c r="D507" t="s">
+        <v>505</v>
+      </c>
+      <c r="E507" t="s">
+        <v>15</v>
       </c>
       <c r="F507" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testDeleteButton</v>
       </c>
       <c r="G507" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="508" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testDeleteButton"</v>
+      </c>
+    </row>
+    <row r="508" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>484</v>
+        <v>512</v>
       </c>
       <c r="B508" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>LoginForm.vue</v>
       </c>
       <c r="C508" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E508" t="str">
-        <f>IF(COUNTIF(C$2:C507,C508)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\LoginForm.vuelogin_text</v>
+      </c>
+      <c r="D508" t="s">
+        <v>513</v>
+      </c>
+      <c r="E508" t="s">
+        <v>92</v>
       </c>
       <c r="F508" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testLoginTextContent</v>
       </c>
       <c r="G508" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="509" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testLoginTextContent"</v>
+      </c>
+    </row>
+    <row r="509" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>484</v>
+        <v>512</v>
       </c>
       <c r="B509" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>LoginForm.vue</v>
       </c>
       <c r="C509" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E509" t="str">
-        <f>IF(COUNTIF(C$2:C508,C509)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\LoginForm.vuesignin_text</v>
+      </c>
+      <c r="D509" t="s">
+        <v>514</v>
+      </c>
+      <c r="E509" t="s">
+        <v>92</v>
       </c>
       <c r="F509" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testSigninTextContent</v>
       </c>
       <c r="G509" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="510" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSigninTextContent"</v>
+      </c>
+    </row>
+    <row r="510" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>484</v>
+        <v>512</v>
       </c>
       <c r="B510" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>LoginForm.vue</v>
       </c>
       <c r="C510" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E510" t="str">
-        <f>IF(COUNTIF(C$2:C509,C510)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\LoginForm.vueemail</v>
+      </c>
+      <c r="D510" t="s">
+        <v>421</v>
+      </c>
+      <c r="E510" t="s">
+        <v>68</v>
       </c>
       <c r="F510" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testEmailTextInput</v>
       </c>
       <c r="G510" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="511" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testEmailTextInput"</v>
+      </c>
+    </row>
+    <row r="511" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>484</v>
+        <v>512</v>
       </c>
       <c r="B511" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>LoginForm.vue</v>
       </c>
       <c r="C511" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E511" t="str">
-        <f>IF(COUNTIF(C$2:C510,C511)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\LoginForm.vuepassword</v>
+      </c>
+      <c r="D511" t="s">
+        <v>515</v>
+      </c>
+      <c r="E511" t="s">
+        <v>68</v>
       </c>
       <c r="F511" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testPasswordTextInput</v>
       </c>
       <c r="G511" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="512" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testPasswordTextInput"</v>
+      </c>
+    </row>
+    <row r="512" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>484</v>
+        <v>512</v>
       </c>
       <c r="B512" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>LoginForm.vue</v>
       </c>
       <c r="C512" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E512" t="str">
-        <f>IF(COUNTIF(C$2:C511,C512)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\LoginForm.vuerequest_password_reset</v>
+      </c>
+      <c r="D512" t="s">
+        <v>516</v>
+      </c>
+      <c r="E512" t="s">
+        <v>91</v>
       </c>
       <c r="F512" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testRequestPasswordResetLink</v>
       </c>
       <c r="G512" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="513" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testRequestPasswordResetLink"</v>
+      </c>
+    </row>
+    <row r="513" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>484</v>
+        <v>512</v>
       </c>
       <c r="B513" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>LoginForm.vue</v>
       </c>
       <c r="C513" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E513" t="str">
-        <f>IF(COUNTIF(C$2:C512,C513)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\LoginForm.vuelogin</v>
+      </c>
+      <c r="D513" t="s">
+        <v>517</v>
+      </c>
+      <c r="E513" t="s">
+        <v>15</v>
       </c>
       <c r="F513" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testLoginButton</v>
       </c>
       <c r="G513" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="514" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testLoginButton"</v>
+      </c>
+    </row>
+    <row r="514" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>484</v>
+        <v>512</v>
       </c>
       <c r="B514" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>LoginForm.vue</v>
       </c>
       <c r="C514" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E514" t="str">
-        <f>IF(COUNTIF(C$2:C513,C514)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\LoginForm.vuerequest_access</v>
+      </c>
+      <c r="D514" t="s">
+        <v>518</v>
+      </c>
+      <c r="E514" t="s">
+        <v>15</v>
       </c>
       <c r="F514" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testRequestAccessButton</v>
       </c>
       <c r="G514" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="515" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testRequestAccessButton"</v>
+      </c>
+    </row>
+    <row r="515" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>484</v>
+        <v>519</v>
       </c>
       <c r="B515" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Modal.vue</v>
       </c>
       <c r="C515" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E515" t="str">
-        <f>IF(COUNTIF(C$2:C514,C515)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Modal.vuemodalCancel</v>
+      </c>
+      <c r="D515" t="s">
+        <v>520</v>
+      </c>
+      <c r="E515" t="s">
+        <v>93</v>
       </c>
       <c r="F515" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testModalCancelIcon</v>
       </c>
       <c r="G515" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="516" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testModalCancelIcon"</v>
+      </c>
+    </row>
+    <row r="516" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>484</v>
+        <v>519</v>
       </c>
       <c r="B516" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Modal.vue</v>
       </c>
       <c r="C516" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E516" t="str">
-        <f>IF(COUNTIF(C$2:C515,C516)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Modal.vuemodalCancel2</v>
+      </c>
+      <c r="D516" t="s">
+        <v>521</v>
+      </c>
+      <c r="E516" t="s">
+        <v>93</v>
       </c>
       <c r="F516" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testModalCancel2Icon</v>
       </c>
       <c r="G516" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="517" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testModalCancel2Icon"</v>
+      </c>
+    </row>
+    <row r="517" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>484</v>
+        <v>519</v>
       </c>
       <c r="B517" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Modal.vue</v>
       </c>
       <c r="C517" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E517" t="str">
-        <f>IF(COUNTIF(C$2:C516,C517)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Modal.vuemodalOk</v>
+      </c>
+      <c r="D517" t="s">
+        <v>522</v>
+      </c>
+      <c r="E517" t="s">
+        <v>15</v>
       </c>
       <c r="F517" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testModalOkButton</v>
       </c>
       <c r="G517" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="518" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testModalOkButton"</v>
+      </c>
+    </row>
+    <row r="518" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>484</v>
+        <v>523</v>
       </c>
       <c r="B518" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>PdfViewer.vue</v>
       </c>
       <c r="C518" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E518" t="str">
-        <f>IF(COUNTIF(C$2:C517,C518)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\PdfViewer.vuedownload</v>
+      </c>
+      <c r="D518" t="s">
+        <v>368</v>
+      </c>
+      <c r="E518" t="s">
+        <v>91</v>
       </c>
       <c r="F518" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testDownloadLink</v>
       </c>
       <c r="G518" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="519" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testDownloadLink"</v>
+      </c>
+    </row>
+    <row r="519" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>484</v>
+        <v>524</v>
       </c>
       <c r="B519" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>OrganizationSearchInput.vue</v>
       </c>
       <c r="C519" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E519" t="str">
-        <f>IF(COUNTIF(C$2:C518,C519)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\OrganizationSearchInput.vueorganization_name</v>
+      </c>
+      <c r="D519" t="s">
+        <v>525</v>
+      </c>
+      <c r="E519" t="s">
+        <v>87</v>
       </c>
       <c r="F519" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testOrganizationNameSelect</v>
       </c>
       <c r="G519" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="520" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testOrganizationNameSelect"</v>
+      </c>
+    </row>
+    <row r="520" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="B520" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>RecurringSchedule.vue</v>
       </c>
       <c r="C520" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E520" t="str">
-        <f>IF(COUNTIF(C$2:C519,C520)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RecurringSchedule.vueschedule_frequency</v>
+      </c>
+      <c r="D520" t="s">
+        <v>527</v>
+      </c>
+      <c r="E520" t="s">
+        <v>87</v>
       </c>
       <c r="F520" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testScheduleFrequencySelect</v>
       </c>
       <c r="G520" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="521" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testScheduleFrequencySelect"</v>
+      </c>
+    </row>
+    <row r="521" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="B521" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>RecurringSchedule.vue</v>
       </c>
       <c r="C521" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E521" t="str">
-        <f>IF(COUNTIF(C$2:C520,C521)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RecurringSchedule.vuedailyOption</v>
+      </c>
+      <c r="D521" t="s">
+        <v>528</v>
+      </c>
+      <c r="E521" t="s">
+        <v>70</v>
       </c>
       <c r="F521" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testDailyOptionRadio</v>
       </c>
       <c r="G521" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="522" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testDailyOptionRadio"</v>
+      </c>
+    </row>
+    <row r="522" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="B522" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>RecurringSchedule.vue</v>
       </c>
       <c r="C522" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E522" t="str">
-        <f>IF(COUNTIF(C$2:C521,C522)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RecurringSchedule.vuedayInterval</v>
+      </c>
+      <c r="D522" t="s">
+        <v>529</v>
+      </c>
+      <c r="E522" t="s">
+        <v>68</v>
       </c>
       <c r="F522" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testDayIntervalTextInput</v>
       </c>
       <c r="G522" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="523" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testDayIntervalTextInput"</v>
+      </c>
+    </row>
+    <row r="523" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="B523" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>RecurringSchedule.vue</v>
       </c>
       <c r="C523" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E523" t="str">
-        <f>IF(COUNTIF(C$2:C522,C523)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RecurringSchedule.vueevery_weekday_interval</v>
+      </c>
+      <c r="D523" t="s">
+        <v>530</v>
+      </c>
+      <c r="E523" t="s">
+        <v>70</v>
       </c>
       <c r="F523" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testEveryWeekdayIntervalRadio</v>
       </c>
       <c r="G523" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="524" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testEveryWeekdayIntervalRadio"</v>
+      </c>
+    </row>
+    <row r="524" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="B524" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>RecurringSchedule.vue</v>
       </c>
       <c r="C524" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E524" t="str">
-        <f>IF(COUNTIF(C$2:C523,C524)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RecurringSchedule.vuecalendar</v>
+      </c>
+      <c r="D524" t="s">
+        <v>531</v>
+      </c>
+      <c r="E524" t="s">
+        <v>93</v>
       </c>
       <c r="F524" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testCalendarIcon</v>
       </c>
       <c r="G524" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="525" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testCalendarIcon"</v>
+      </c>
+    </row>
+    <row r="525" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="B525" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>RecurringSchedule.vue</v>
       </c>
       <c r="C525" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E525" t="str">
-        <f>IF(COUNTIF(C$2:C524,C525)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RecurringSchedule.vueendDatePicker</v>
+      </c>
+      <c r="D525" t="s">
+        <v>532</v>
+      </c>
+      <c r="E525" t="s">
+        <v>307</v>
       </c>
       <c r="F525" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testEndDatePickerInput</v>
       </c>
       <c r="G525" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="526" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testEndDatePickerInput"</v>
+      </c>
+    </row>
+    <row r="526" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="B526" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>RecurringSchedule.vue</v>
       </c>
       <c r="C526" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E526" t="str">
-        <f>IF(COUNTIF(C$2:C525,C526)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RecurringSchedule.vueadd_schedule</v>
+      </c>
+      <c r="D526" t="s">
+        <v>533</v>
+      </c>
+      <c r="E526" t="s">
+        <v>15</v>
       </c>
       <c r="F526" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testAddScheduleButton</v>
       </c>
       <c r="G526" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="527" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testAddScheduleButton"</v>
+      </c>
+    </row>
+    <row r="527" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>484</v>
+        <v>535</v>
       </c>
       <c r="B527" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>RequestRedeploy.vue</v>
       </c>
       <c r="C527" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E527" t="str">
-        <f>IF(COUNTIF(C$2:C526,C527)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RequestRedeploy.vueselect_incident</v>
+      </c>
+      <c r="D527" t="s">
+        <v>211</v>
+      </c>
+      <c r="E527" t="s">
+        <v>87</v>
       </c>
       <c r="F527" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testSelectIncidentSelect</v>
       </c>
       <c r="G527" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="528" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testSelectIncidentSelect"</v>
+      </c>
+    </row>
+    <row r="528" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>484</v>
+        <v>535</v>
       </c>
       <c r="B528" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>RequestRedeploy.vue</v>
       </c>
       <c r="C528" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E528" t="str">
-        <f>IF(COUNTIF(C$2:C527,C528)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\RequestRedeploy.vuerequestIncident</v>
+      </c>
+      <c r="D528" t="s">
+        <v>534</v>
+      </c>
+      <c r="E528" t="s">
+        <v>15</v>
       </c>
       <c r="F528" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testRequestIncidentButton</v>
       </c>
       <c r="G528" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="529" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testRequestIncidentButton"</v>
+      </c>
+    </row>
+    <row r="529" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>484</v>
+        <v>536</v>
       </c>
       <c r="B529" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>SimpleMap.vue</v>
       </c>
       <c r="C529" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E529" t="str">
-        <f>IF(COUNTIF(C$2:C528,C529)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\SimpleMap.vuezoom_in</v>
+      </c>
+      <c r="D529" t="s">
+        <v>541</v>
+      </c>
+      <c r="E529" t="s">
+        <v>15</v>
       </c>
       <c r="F529" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testZoomInButton</v>
       </c>
       <c r="G529" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="530" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testZoomInButton"</v>
+      </c>
+    </row>
+    <row r="530" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>484</v>
+        <v>536</v>
       </c>
       <c r="B530" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>SimpleMap.vue</v>
       </c>
       <c r="C530" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E530" t="str">
-        <f>IF(COUNTIF(C$2:C529,C530)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\SimpleMap.vuezoom_out</v>
+      </c>
+      <c r="D530" t="s">
+        <v>537</v>
+      </c>
+      <c r="E530" t="s">
+        <v>15</v>
       </c>
       <c r="F530" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testZoomOutButton</v>
       </c>
       <c r="G530" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="531" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testZoomOutButton"</v>
+      </c>
+    </row>
+    <row r="531" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>484</v>
+        <v>536</v>
       </c>
       <c r="B531" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>SimpleMap.vue</v>
       </c>
       <c r="C531" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E531" t="str">
-        <f>IF(COUNTIF(C$2:C530,C531)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\SimpleMap.vuezoom_to_make_interactive</v>
+      </c>
+      <c r="D531" t="s">
+        <v>538</v>
+      </c>
+      <c r="E531" t="s">
+        <v>15</v>
       </c>
       <c r="F531" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testZoomToMakeInteractiveButton</v>
       </c>
       <c r="G531" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="532" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testZoomToMakeInteractiveButton"</v>
+      </c>
+    </row>
+    <row r="532" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>484</v>
+        <v>536</v>
       </c>
       <c r="B532" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>SimpleMap.vue</v>
       </c>
       <c r="C532" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E532" t="str">
-        <f>IF(COUNTIF(C$2:C531,C532)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\SimpleMap.vuezoom_to_incident</v>
+      </c>
+      <c r="D532" t="s">
+        <v>539</v>
+      </c>
+      <c r="E532" t="s">
+        <v>15</v>
       </c>
       <c r="F532" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testZoomToIncidentButton</v>
       </c>
       <c r="G532" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-    </row>
-    <row r="533" spans="1:7" x14ac:dyDescent="0.25">
+        <v>data-testid="testZoomToIncidentButton"</v>
+      </c>
+    </row>
+    <row r="533" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>484</v>
+        <v>536</v>
       </c>
       <c r="B533" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>SimpleMap.vue</v>
       </c>
       <c r="C533" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E533" t="str">
-        <f>IF(COUNTIF(C$2:C532,C533)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\SimpleMap.vueshowLegend</v>
+      </c>
+      <c r="D533" t="s">
+        <v>540</v>
+      </c>
+      <c r="E533" t="s">
+        <v>69</v>
       </c>
       <c r="F533" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testShowLegendDiv</v>
       </c>
       <c r="G533" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="testShowLegendDiv"</v>
       </c>
     </row>
     <row r="534" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>484</v>
+        <v>545</v>
       </c>
       <c r="B534" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Slider.vue</v>
       </c>
       <c r="C534" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E534" t="str">
-        <f>IF(COUNTIF(C$2:C533,C534)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Slider.vue:several_calculated</v>
+      </c>
+      <c r="D534" t="s">
+        <v>104</v>
       </c>
       <c r="F534" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>test:SeveralCalculated</v>
       </c>
       <c r="G534" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="test:SeveralCalculated"</v>
       </c>
     </row>
     <row r="535" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>484</v>
+        <v>542</v>
       </c>
       <c r="B535" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>DisasterIcon.vue</v>
       </c>
       <c r="C535" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E535" t="str">
-        <f>IF(COUNTIF(C$2:C534,C535)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\DisasterIcon.vuerandomEasterEgg</v>
+      </c>
+      <c r="D535" t="s">
+        <v>543</v>
+      </c>
+      <c r="E535" t="s">
+        <v>93</v>
       </c>
       <c r="F535" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testRandomEasterEggIcon</v>
       </c>
       <c r="G535" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="testRandomEasterEggIcon"</v>
       </c>
     </row>
     <row r="536" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>484</v>
+        <v>542</v>
       </c>
       <c r="B536" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>DisasterIcon.vue</v>
       </c>
       <c r="C536" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E536" t="str">
-        <f>IF(COUNTIF(C$2:C535,C536)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\DisasterIcon.vueincidentImage</v>
+      </c>
+      <c r="D536" t="s">
+        <v>544</v>
+      </c>
+      <c r="E536" t="s">
+        <v>93</v>
       </c>
       <c r="F536" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testIncidentImageIcon</v>
       </c>
       <c r="G536" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="testIncidentImageIcon"</v>
       </c>
     </row>
     <row r="537" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>484</v>
+        <v>546</v>
       </c>
       <c r="B537" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Tag.vue</v>
       </c>
       <c r="C537" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E537" t="str">
-        <f>IF(COUNTIF(C$2:C536,C537)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Tag.vuecancel</v>
+      </c>
+      <c r="D537" t="s">
+        <v>40</v>
+      </c>
+      <c r="E537" t="s">
+        <v>93</v>
       </c>
       <c r="F537" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testCancelIcon</v>
       </c>
       <c r="G537" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="testCancelIcon"</v>
       </c>
     </row>
     <row r="538" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>484</v>
+        <v>547</v>
       </c>
       <c r="B538" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Table.vue</v>
       </c>
       <c r="C538" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E538" t="str">
-        <f>IF(COUNTIF(C$2:C537,C538)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Table.vuesetAllChecked</v>
+      </c>
+      <c r="D538" t="s">
+        <v>548</v>
+      </c>
+      <c r="E538" t="s">
+        <v>66</v>
       </c>
       <c r="F538" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testSetAllCheckedCheckbox</v>
       </c>
       <c r="G538" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="testSetAllCheckedCheckbox"</v>
       </c>
     </row>
     <row r="539" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>484</v>
+        <v>547</v>
       </c>
       <c r="B539" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Table.vue</v>
       </c>
       <c r="C539" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Table.vue:several_calculated</v>
+      </c>
+      <c r="D539" t="s">
+        <v>104</v>
       </c>
       <c r="E539" t="str">
         <f>IF(COUNTIF(C$2:C538,C539)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F539" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>test:SeveralCalculated</v>
       </c>
       <c r="G539" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="test:SeveralCalculated"</v>
       </c>
     </row>
     <row r="540" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>484</v>
+        <v>547</v>
       </c>
       <c r="B540" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Table.vue</v>
       </c>
       <c r="C540" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E540" t="str">
-        <f>IF(COUNTIF(C$2:C539,C540)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Table.vueno_items_found</v>
+      </c>
+      <c r="D540" t="s">
+        <v>549</v>
+      </c>
+      <c r="E540" t="s">
+        <v>69</v>
       </c>
       <c r="F540" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testNoItemsFoundDiv</v>
       </c>
       <c r="G540" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="testNoItemsFoundDiv"</v>
       </c>
     </row>
     <row r="541" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>484</v>
+        <v>547</v>
       </c>
       <c r="B541" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Table.vue</v>
       </c>
       <c r="C541" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E541" t="str">
-        <f>IF(COUNTIF(C$2:C540,C541)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Table.vuepagination.pageSize</v>
+      </c>
+      <c r="D541" t="s">
+        <v>550</v>
+      </c>
+      <c r="E541" t="s">
+        <v>87</v>
       </c>
       <c r="F541" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testPaginationPagesizeSelect</v>
       </c>
       <c r="G541" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="testPaginationPagesizeSelect"</v>
       </c>
     </row>
     <row r="542" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>484</v>
+        <v>547</v>
       </c>
       <c r="B542" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Table.vue</v>
       </c>
       <c r="C542" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E542" t="str">
-        <f>IF(COUNTIF(C$2:C541,C542)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Table.vuepagination.prev</v>
+      </c>
+      <c r="D542" t="s">
+        <v>551</v>
+      </c>
+      <c r="E542" t="s">
+        <v>15</v>
       </c>
       <c r="F542" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testPaginationPrevButton</v>
       </c>
       <c r="G542" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="testPaginationPrevButton"</v>
       </c>
     </row>
     <row r="543" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>484</v>
+        <v>547</v>
       </c>
       <c r="B543" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v>Table.vue</v>
       </c>
       <c r="C543" t="str">
         <f t="shared" si="34"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\</v>
-      </c>
-      <c r="E543" t="str">
-        <f>IF(COUNTIF(C$2:C542,C543)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\components\Table.vuepagination.next</v>
+      </c>
+      <c r="D543" t="s">
+        <v>552</v>
+      </c>
+      <c r="E543" t="s">
+        <v>15</v>
       </c>
       <c r="F543" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>testPaginationNextButton</v>
       </c>
       <c r="G543" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>data-testid="testPaginationNextButton"</v>
       </c>
     </row>
     <row r="544" spans="1:7" x14ac:dyDescent="0.25">
@@ -16408,7 +16716,7 @@
       </c>
       <c r="E544" t="str">
         <f>IF(COUNTIF(C$2:C543,C544)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F544" t="str">
         <f t="shared" si="35"/>

</xml_diff>

<commit_message>
Add missing alt text to icons
(cherry picked from commit 37d497dd28d32299aeb298f97dbb111958e3b5ff)
</commit_message>
<xml_diff>
--- a/test/e2e/List of data-testids.xlsx
+++ b/test/e2e/List of data-testids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\test\e2e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CF4252-6E9D-49CF-961A-28454BD06CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5365B592-6F80-4577-9AF1-84C70A519063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2190" yWindow="1215" windowWidth="24330" windowHeight="12585" xr2:uid="{51F30F27-9EA9-4B4D-86A3-E32FA30758F4}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2672" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2708" uniqueCount="869">
   <si>
     <t>Output</t>
   </si>
@@ -2260,9 +2260,6 @@
     <t>ccu_during_covid_iframe</t>
   </si>
   <si>
-    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</t>
-  </si>
-  <si>
     <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Affiliates.vue</t>
   </si>
   <si>
@@ -2606,6 +2603,39 @@
   </si>
   <si>
     <t>user_invited_by_results</t>
+  </si>
+  <si>
+    <t>user_profile_picture</t>
+  </si>
+  <si>
+    <t>user_email</t>
+  </si>
+  <si>
+    <t>user_chat</t>
+  </si>
+  <si>
+    <t>user_call</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserView.vue</t>
+  </si>
+  <si>
+    <t>user_view</t>
+  </si>
+  <si>
+    <t>remove_user</t>
+  </si>
+  <si>
+    <t>user_details</t>
+  </si>
+  <si>
+    <t>user_roles</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</t>
+  </si>
+  <si>
+    <t>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\PhoneSystem.vue</t>
   </si>
 </sst>
 </file>
@@ -2960,8 +2990,8 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A892" sqref="A892"/>
+      <pane ySplit="1" topLeftCell="A896" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B911" sqref="B911"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2994,7 +3024,7 @@
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -22897,7 +22927,7 @@
     </row>
     <row r="739" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B739" t="str">
         <f t="shared" si="45"/>
@@ -22908,7 +22938,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Affiliates.vueadd_affiliate</v>
       </c>
       <c r="D739" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E739" t="s">
         <v>15</v>
@@ -22924,7 +22954,7 @@
     </row>
     <row r="740" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B740" t="str">
         <f t="shared" si="45"/>
@@ -22935,7 +22965,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Affiliates.vuerequest_affiliate</v>
       </c>
       <c r="D740" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E740" t="s">
         <v>98</v>
@@ -22951,7 +22981,7 @@
     </row>
     <row r="741" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B741" t="str">
         <f t="shared" si="45"/>
@@ -22962,7 +22992,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Affiliates.vueselectedAffiliate</v>
       </c>
       <c r="D741" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E741" t="s">
         <v>216</v>
@@ -22978,7 +23008,7 @@
     </row>
     <row r="742" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B742" t="str">
         <f t="shared" si="45"/>
@@ -22989,10 +23019,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Affiliates.vuerequest_reason</v>
       </c>
       <c r="D742" t="s">
+        <v>747</v>
+      </c>
+      <c r="E742" t="s">
         <v>748</v>
-      </c>
-      <c r="E742" t="s">
-        <v>749</v>
       </c>
       <c r="F742" t="str">
         <f t="shared" si="47"/>
@@ -23005,7 +23035,7 @@
     </row>
     <row r="743" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B743" t="str">
         <f t="shared" si="45"/>
@@ -23032,7 +23062,7 @@
     </row>
     <row r="744" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B744" t="str">
         <f t="shared" si="45"/>
@@ -23043,7 +23073,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Affiliates.vueinvite</v>
       </c>
       <c r="D744" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E744" t="s">
         <v>15</v>
@@ -23059,7 +23089,7 @@
     </row>
     <row r="745" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B745" t="str">
         <f t="shared" si="45"/>
@@ -23070,7 +23100,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Affiliates.vueaffiliates</v>
       </c>
       <c r="D745" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E745" t="s">
         <v>268</v>
@@ -23086,7 +23116,7 @@
     </row>
     <row r="746" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B746" t="str">
         <f t="shared" si="45"/>
@@ -23097,7 +23127,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Affiliates.vueunaffiliate</v>
       </c>
       <c r="D746" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E746" t="s">
         <v>15</v>
@@ -23113,7 +23143,7 @@
     </row>
     <row r="747" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B747" t="str">
         <f t="shared" si="45"/>
@@ -23140,7 +23170,7 @@
     </row>
     <row r="748" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B748" t="str">
         <f t="shared" si="45"/>
@@ -23167,7 +23197,7 @@
     </row>
     <row r="749" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B749" t="str">
         <f t="shared" si="45"/>
@@ -23195,7 +23225,7 @@
     </row>
     <row r="750" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B750" t="str">
         <f t="shared" si="45"/>
@@ -23206,7 +23236,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vuecreate_team</v>
       </c>
       <c r="D750" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E750" t="s">
         <v>98</v>
@@ -23222,7 +23252,7 @@
     </row>
     <row r="751" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B751" t="str">
         <f t="shared" si="45"/>
@@ -23233,7 +23263,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vueteam_name</v>
       </c>
       <c r="D751" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E751" t="s">
         <v>68</v>
@@ -23249,7 +23279,7 @@
     </row>
     <row r="752" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B752" t="str">
         <f t="shared" si="45"/>
@@ -23260,7 +23290,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vuesuggest_name</v>
       </c>
       <c r="D752" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E752" t="s">
         <v>15</v>
@@ -23276,7 +23306,7 @@
     </row>
     <row r="753" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B753" t="str">
         <f t="shared" si="45"/>
@@ -23287,10 +23317,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vueteam.users</v>
       </c>
       <c r="D753" t="s">
+        <v>756</v>
+      </c>
+      <c r="E753" t="s">
         <v>757</v>
-      </c>
-      <c r="E753" t="s">
-        <v>758</v>
       </c>
       <c r="F753" t="str">
         <f t="shared" si="50"/>
@@ -23303,7 +23333,7 @@
     </row>
     <row r="754" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B754" t="str">
         <f t="shared" si="45"/>
@@ -23314,7 +23344,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vueteam.users.drag</v>
       </c>
       <c r="D754" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E754" t="s">
         <v>93</v>
@@ -23330,7 +23360,7 @@
     </row>
     <row r="755" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B755" t="str">
         <f t="shared" si="45"/>
@@ -23341,7 +23371,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vueadd_members</v>
       </c>
       <c r="D755" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E755" t="s">
         <v>15</v>
@@ -23357,7 +23387,7 @@
     </row>
     <row r="756" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B756" t="str">
         <f t="shared" si="45"/>
@@ -23368,10 +23398,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vueteamWorksites</v>
       </c>
       <c r="D756" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E756" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F756" t="str">
         <f t="shared" si="50"/>
@@ -23384,7 +23414,7 @@
     </row>
     <row r="757" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B757" t="str">
         <f t="shared" si="45"/>
@@ -23395,7 +23425,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vueworksites.drag</v>
       </c>
       <c r="D757" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E757" t="s">
         <v>93</v>
@@ -23411,7 +23441,7 @@
     </row>
     <row r="758" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B758" t="str">
         <f t="shared" ref="B758:B821" si="52">IF(A758="","",MID(A758,FIND("@",SUBSTITUTE(A758,"\","@",LEN(A758)-LEN(SUBSTITUTE(A758,"\",""))))+1,LEN(A758)))</f>
@@ -23422,7 +23452,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vueassign_cases</v>
       </c>
       <c r="D758" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E758" t="s">
         <v>15</v>
@@ -23438,7 +23468,7 @@
     </row>
     <row r="759" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B759" t="str">
         <f t="shared" si="52"/>
@@ -23449,7 +23479,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vuesearch_drag_members</v>
       </c>
       <c r="D759" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E759" t="s">
         <v>216</v>
@@ -23465,7 +23495,7 @@
     </row>
     <row r="760" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B760" t="str">
         <f t="shared" si="52"/>
@@ -23476,10 +23506,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vueusersList</v>
       </c>
       <c r="D760" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E760" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F760" t="str">
         <f t="shared" si="50"/>
@@ -23492,7 +23522,7 @@
     </row>
     <row r="761" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B761" t="str">
         <f t="shared" si="52"/>
@@ -23503,7 +23533,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vuecurrentCaseSearch</v>
       </c>
       <c r="D761" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E761" t="s">
         <v>216</v>
@@ -23519,7 +23549,7 @@
     </row>
     <row r="762" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B762" t="str">
         <f t="shared" si="52"/>
@@ -23530,10 +23560,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\CreateTeamModal.vueworksites</v>
       </c>
       <c r="D762" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E762" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F762" t="str">
         <f t="shared" si="50"/>
@@ -23546,7 +23576,7 @@
     </row>
     <row r="763" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B763" t="str">
         <f t="shared" si="52"/>
@@ -23573,7 +23603,7 @@
     </row>
     <row r="764" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B764" t="str">
         <f t="shared" si="52"/>
@@ -23600,7 +23630,7 @@
     </row>
     <row r="765" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B765" t="str">
         <f t="shared" si="52"/>
@@ -23611,7 +23641,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Invitations.vueexportInvitationRequests</v>
       </c>
       <c r="D765" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E765" t="s">
         <v>15</v>
@@ -23631,7 +23661,7 @@
     </row>
     <row r="766" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B766" t="str">
         <f t="shared" si="52"/>
@@ -23642,7 +23672,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Invitations.vueinvitationRequests</v>
       </c>
       <c r="D766" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E766" t="s">
         <v>268</v>
@@ -23662,7 +23692,7 @@
     </row>
     <row r="767" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B767" t="str">
         <f t="shared" si="52"/>
@@ -23673,7 +23703,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Invitations.vueignore</v>
       </c>
       <c r="D767" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E767" t="s">
         <v>15</v>
@@ -23693,7 +23723,7 @@
     </row>
     <row r="768" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A768" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B768" t="str">
         <f t="shared" si="52"/>
@@ -23724,7 +23754,7 @@
     </row>
     <row r="769" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B769" t="str">
         <f t="shared" si="52"/>
@@ -23755,7 +23785,7 @@
     </row>
     <row r="770" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B770" t="str">
         <f t="shared" si="52"/>
@@ -23766,7 +23796,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Invitations.vueexportInvitations</v>
       </c>
       <c r="D770" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E770" t="s">
         <v>15</v>
@@ -23786,7 +23816,7 @@
     </row>
     <row r="771" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B771" t="str">
         <f t="shared" si="52"/>
@@ -23797,7 +23827,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Invitations.vuedeleteExpiredInvitations</v>
       </c>
       <c r="D771" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E771" t="s">
         <v>15</v>
@@ -23817,7 +23847,7 @@
     </row>
     <row r="772" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B772" t="str">
         <f t="shared" si="52"/>
@@ -23849,7 +23879,7 @@
     </row>
     <row r="773" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B773" t="str">
         <f t="shared" si="52"/>
@@ -23880,7 +23910,7 @@
     </row>
     <row r="774" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B774" t="str">
         <f t="shared" si="52"/>
@@ -23911,7 +23941,7 @@
     </row>
     <row r="775" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B775" t="str">
         <f t="shared" si="52"/>
@@ -23922,7 +23952,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Invitations.vuedelete_invitation</v>
       </c>
       <c r="D775" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E775" t="s">
         <v>15</v>
@@ -23942,7 +23972,7 @@
     </row>
     <row r="776" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B776" t="str">
         <f t="shared" si="52"/>
@@ -23953,7 +23983,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Layers.vuegetLocations</v>
       </c>
       <c r="D776" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E776" t="s">
         <v>216</v>
@@ -23973,7 +24003,7 @@
     </row>
     <row r="777" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B777" t="str">
         <f t="shared" si="52"/>
@@ -23984,7 +24014,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Layers.vuelocationTypeFilter</v>
       </c>
       <c r="D777" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E777" t="s">
         <v>87</v>
@@ -24004,7 +24034,7 @@
     </row>
     <row r="778" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B778" t="str">
         <f t="shared" si="52"/>
@@ -24015,7 +24045,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Layers.vuecreate_location</v>
       </c>
       <c r="D778" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E778" t="s">
         <v>15</v>
@@ -24035,7 +24065,7 @@
     </row>
     <row r="779" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B779" t="str">
         <f t="shared" si="52"/>
@@ -24046,7 +24076,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Layers.vuelocations</v>
       </c>
       <c r="D779" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E779" t="s">
         <v>268</v>
@@ -24066,7 +24096,7 @@
     </row>
     <row r="780" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B780" t="str">
         <f t="shared" si="52"/>
@@ -24097,7 +24127,7 @@
     </row>
     <row r="781" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B781" t="str">
         <f t="shared" si="52"/>
@@ -24108,7 +24138,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\InviteUsers.vueshowInvite</v>
       </c>
       <c r="D781" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E781" t="s">
         <v>98</v>
@@ -24128,7 +24158,7 @@
     </row>
     <row r="782" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B782" t="str">
         <f t="shared" si="52"/>
@@ -24139,7 +24169,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\InviteUsers.vueusersToInvite</v>
       </c>
       <c r="D782" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E782" t="s">
         <v>68</v>
@@ -24159,7 +24189,7 @@
     </row>
     <row r="783" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B783" t="str">
         <f t="shared" si="52"/>
@@ -24190,7 +24220,7 @@
     </row>
     <row r="784" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B784" t="str">
         <f t="shared" si="52"/>
@@ -24221,7 +24251,7 @@
     </row>
     <row r="785" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B785" t="str">
         <f t="shared" si="52"/>
@@ -24252,7 +24282,7 @@
     </row>
     <row r="786" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B786" t="str">
         <f t="shared" si="52"/>
@@ -24283,7 +24313,7 @@
     </row>
     <row r="787" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B787" t="str">
         <f t="shared" si="52"/>
@@ -24314,7 +24344,7 @@
     </row>
     <row r="788" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B788" t="str">
         <f t="shared" si="52"/>
@@ -24345,7 +24375,7 @@
     </row>
     <row r="789" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B789" t="str">
         <f t="shared" si="52"/>
@@ -24376,7 +24406,7 @@
     </row>
     <row r="790" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B790" t="str">
         <f t="shared" si="52"/>
@@ -24407,7 +24437,7 @@
     </row>
     <row r="791" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B791" t="str">
         <f t="shared" si="52"/>
@@ -24438,7 +24468,7 @@
     </row>
     <row r="792" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B792" t="str">
         <f t="shared" si="52"/>
@@ -24469,7 +24499,7 @@
     </row>
     <row r="793" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B793" t="str">
         <f t="shared" si="52"/>
@@ -24500,7 +24530,7 @@
     </row>
     <row r="794" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B794" t="str">
         <f t="shared" si="52"/>
@@ -24531,7 +24561,7 @@
     </row>
     <row r="795" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B795" t="str">
         <f t="shared" si="52"/>
@@ -24562,7 +24592,7 @@
     </row>
     <row r="796" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B796" t="str">
         <f t="shared" si="52"/>
@@ -24593,7 +24623,7 @@
     </row>
     <row r="797" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B797" t="str">
         <f t="shared" si="52"/>
@@ -24624,7 +24654,7 @@
     </row>
     <row r="798" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B798" t="str">
         <f t="shared" si="52"/>
@@ -24655,7 +24685,7 @@
     </row>
     <row r="799" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B799" t="str">
         <f t="shared" si="52"/>
@@ -24687,7 +24717,7 @@
     </row>
     <row r="800" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B800" t="str">
         <f t="shared" si="52"/>
@@ -24718,7 +24748,7 @@
     </row>
     <row r="801" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B801" t="str">
         <f t="shared" si="52"/>
@@ -24729,7 +24759,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueadd_primary_contacts</v>
       </c>
       <c r="D801" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E801" t="s">
         <v>216</v>
@@ -24749,7 +24779,7 @@
     </row>
     <row r="802" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B802" t="str">
         <f t="shared" si="52"/>
@@ -24780,7 +24810,7 @@
     </row>
     <row r="803" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B803" t="str">
         <f t="shared" si="52"/>
@@ -24811,7 +24841,7 @@
     </row>
     <row r="804" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B804" t="str">
         <f t="shared" si="52"/>
@@ -24822,7 +24852,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuedonation_url</v>
       </c>
       <c r="D804" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E804" t="s">
         <v>68</v>
@@ -24842,7 +24872,7 @@
     </row>
     <row r="805" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B805" t="str">
         <f t="shared" si="52"/>
@@ -24853,7 +24883,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuecapabilitiesMatrix</v>
       </c>
       <c r="D805" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E805" t="s">
         <v>307</v>
@@ -24873,7 +24903,7 @@
     </row>
     <row r="806" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B806" t="str">
         <f t="shared" si="52"/>
@@ -24884,7 +24914,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuecurrent_incidents</v>
       </c>
       <c r="D806" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E806" t="s">
         <v>92</v>
@@ -24904,7 +24934,7 @@
     </row>
     <row r="807" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B807" t="str">
         <f t="shared" si="52"/>
@@ -24935,7 +24965,7 @@
     </row>
     <row r="808" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B808" t="str">
         <f t="shared" si="52"/>
@@ -24946,7 +24976,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuepending_incidents</v>
       </c>
       <c r="D808" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E808" t="s">
         <v>69</v>
@@ -24966,7 +24996,7 @@
     </row>
     <row r="809" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B809" t="str">
         <f t="shared" si="52"/>
@@ -24977,7 +25007,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueedit_primary_location</v>
       </c>
       <c r="D809" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E809" t="s">
         <v>15</v>
@@ -24997,7 +25027,7 @@
     </row>
     <row r="810" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B810" t="str">
         <f t="shared" si="52"/>
@@ -25008,7 +25038,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueadd_primary_location</v>
       </c>
       <c r="D810" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E810" t="s">
         <v>15</v>
@@ -25028,7 +25058,7 @@
     </row>
     <row r="811" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B811" t="str">
         <f t="shared" si="52"/>
@@ -25039,7 +25069,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuecontact_help_change_response</v>
       </c>
       <c r="D811" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E811" t="s">
         <v>15</v>
@@ -25059,7 +25089,7 @@
     </row>
     <row r="812" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B812" t="str">
         <f t="shared" si="52"/>
@@ -25070,7 +25100,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueedit_secondary_location</v>
       </c>
       <c r="D812" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E812" t="s">
         <v>15</v>
@@ -25090,7 +25120,7 @@
     </row>
     <row r="813" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B813" t="str">
         <f t="shared" si="52"/>
@@ -25101,7 +25131,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueadd_secondary_location</v>
       </c>
       <c r="D813" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E813" t="s">
         <v>15</v>
@@ -25121,7 +25151,7 @@
     </row>
     <row r="814" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B814" t="str">
         <f t="shared" si="52"/>
@@ -25132,7 +25162,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuecontact_help_change_response2</v>
       </c>
       <c r="D814" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E814" t="s">
         <v>15</v>
@@ -25152,7 +25182,7 @@
     </row>
     <row r="815" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B815" t="str">
         <f t="shared" si="52"/>
@@ -25163,7 +25193,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueselect_location</v>
       </c>
       <c r="D815" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E815" t="s">
         <v>98</v>
@@ -25183,7 +25213,7 @@
     </row>
     <row r="816" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A816" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B816" t="str">
         <f t="shared" si="52"/>
@@ -25214,7 +25244,7 @@
     </row>
     <row r="817" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B817" t="str">
         <f t="shared" si="52"/>
@@ -25225,10 +25255,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuecustom_ops_message</v>
       </c>
       <c r="D817" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E817" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F817" t="str">
         <f t="shared" si="55"/>
@@ -25245,7 +25275,7 @@
     </row>
     <row r="818" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A818" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B818" t="str">
         <f t="shared" si="52"/>
@@ -25256,7 +25286,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueadd_custom_tos</v>
       </c>
       <c r="D818" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E818" t="s">
         <v>68</v>
@@ -25276,7 +25306,7 @@
     </row>
     <row r="819" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B819" t="str">
         <f t="shared" si="52"/>
@@ -25307,7 +25337,7 @@
     </row>
     <row r="820" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A820" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B820" t="str">
         <f t="shared" si="52"/>
@@ -25318,7 +25348,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueterms_of_service</v>
       </c>
       <c r="D820" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E820" t="s">
         <v>3</v>
@@ -25338,7 +25368,7 @@
     </row>
     <row r="821" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A821" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B821" t="str">
         <f t="shared" si="52"/>
@@ -25349,10 +25379,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuecustom_legal_tos</v>
       </c>
       <c r="D821" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E821" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F821" t="str">
         <f t="shared" si="55"/>
@@ -25369,7 +25399,7 @@
     </row>
     <row r="822" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A822" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B822" t="str">
         <f t="shared" ref="B822:B885" si="57">IF(A822="","",MID(A822,FIND("@",SUBSTITUTE(A822,"\","@",LEN(A822)-LEN(SUBSTITUTE(A822,"\",""))))+1,LEN(A822)))</f>
@@ -25380,7 +25410,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueadd_custom_liability</v>
       </c>
       <c r="D822" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E822" t="s">
         <v>307</v>
@@ -25400,7 +25430,7 @@
     </row>
     <row r="823" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A823" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B823" t="str">
         <f t="shared" si="57"/>
@@ -25411,7 +25441,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuedelete_liability_waiver</v>
       </c>
       <c r="D823" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E823" t="s">
         <v>15</v>
@@ -25431,7 +25461,7 @@
     </row>
     <row r="824" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A824" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B824" t="str">
         <f t="shared" si="57"/>
@@ -25442,7 +25472,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueliability_waiver</v>
       </c>
       <c r="D824" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E824" t="s">
         <v>3</v>
@@ -25462,7 +25492,7 @@
     </row>
     <row r="825" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A825" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B825" t="str">
         <f t="shared" si="57"/>
@@ -25473,7 +25503,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vuecustom_survivor_waiver</v>
       </c>
       <c r="D825" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E825" t="s">
         <v>15</v>
@@ -25493,7 +25523,7 @@
     </row>
     <row r="826" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A826" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B826" t="str">
         <f t="shared" si="57"/>
@@ -25504,10 +25534,10 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueadd_survivor_waiver_text</v>
       </c>
       <c r="D826" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E826" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F826" t="str">
         <f t="shared" si="55"/>
@@ -25524,7 +25554,7 @@
     </row>
     <row r="827" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A827" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B827" t="str">
         <f t="shared" si="57"/>
@@ -25535,7 +25565,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueorganization_logo2</v>
       </c>
       <c r="D827" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E827" t="s">
         <v>3</v>
@@ -25555,7 +25585,7 @@
     </row>
     <row r="828" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A828" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B828" t="str">
         <f t="shared" si="57"/>
@@ -25566,7 +25596,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Profile.vueadd_terms</v>
       </c>
       <c r="D828" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E828" t="s">
         <v>15</v>
@@ -25586,7 +25616,7 @@
     </row>
     <row r="829" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B829" t="str">
         <f t="shared" si="57"/>
@@ -25597,7 +25627,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Index.vuemyOrganizationDashboard</v>
       </c>
       <c r="D829" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E829" t="s">
         <v>69</v>
@@ -25617,7 +25647,7 @@
     </row>
     <row r="830" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B830" t="str">
         <f t="shared" si="57"/>
@@ -25628,7 +25658,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Index.vuemyOrganizationNav</v>
       </c>
       <c r="D830" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E830" t="s">
         <v>91</v>
@@ -25648,7 +25678,7 @@
     </row>
     <row r="831" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B831" t="str">
         <f t="shared" si="57"/>
@@ -25680,7 +25710,7 @@
     </row>
     <row r="832" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B832" t="str">
         <f t="shared" si="57"/>
@@ -25711,7 +25741,7 @@
     </row>
     <row r="833" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B833" t="str">
         <f t="shared" si="57"/>
@@ -25722,7 +25752,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuedelete_team</v>
       </c>
       <c r="D833" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E833" t="s">
         <v>93</v>
@@ -25742,7 +25772,7 @@
     </row>
     <row r="834" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B834" t="str">
         <f t="shared" si="57"/>
@@ -25753,7 +25783,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuerename_team</v>
       </c>
       <c r="D834" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E834" t="s">
         <v>93</v>
@@ -25773,7 +25803,7 @@
     </row>
     <row r="835" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B835" t="str">
         <f t="shared" si="57"/>
@@ -25784,7 +25814,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueadd_members</v>
       </c>
       <c r="D835" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E835" t="s">
         <v>15</v>
@@ -25804,7 +25834,7 @@
     </row>
     <row r="836" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B836" t="str">
         <f t="shared" si="57"/>
@@ -25815,7 +25845,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueremove_from_team</v>
       </c>
       <c r="D836" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E836" t="s">
         <v>15</v>
@@ -25835,7 +25865,7 @@
     </row>
     <row r="837" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B837" t="str">
         <f t="shared" si="57"/>
@@ -25846,7 +25876,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueallTeamUsers</v>
       </c>
       <c r="D837" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E837" t="s">
         <v>268</v>
@@ -25866,7 +25896,7 @@
     </row>
     <row r="838" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B838" t="str">
         <f t="shared" si="57"/>
@@ -25897,7 +25927,7 @@
     </row>
     <row r="839" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B839" t="str">
         <f t="shared" si="57"/>
@@ -25929,7 +25959,7 @@
     </row>
     <row r="840" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B840" t="str">
         <f t="shared" si="57"/>
@@ -25940,7 +25970,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueenvelope</v>
       </c>
       <c r="D840" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E840" t="s">
         <v>93</v>
@@ -25960,7 +25990,7 @@
     </row>
     <row r="841" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B841" t="str">
         <f t="shared" si="57"/>
@@ -25991,7 +26021,7 @@
     </row>
     <row r="842" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B842" t="str">
         <f t="shared" si="57"/>
@@ -26002,7 +26032,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueteams.settings</v>
       </c>
       <c r="D842" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E842" t="s">
         <v>93</v>
@@ -26022,7 +26052,7 @@
     </row>
     <row r="843" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B843" t="str">
         <f t="shared" si="57"/>
@@ -26033,7 +26063,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueteams_emails</v>
       </c>
       <c r="D843" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E843" t="s">
         <v>69</v>
@@ -26053,7 +26083,7 @@
     </row>
     <row r="844" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B844" t="str">
         <f t="shared" si="57"/>
@@ -26064,7 +26094,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuemove_to_another_team</v>
       </c>
       <c r="D844" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E844" t="s">
         <v>91</v>
@@ -26084,7 +26114,7 @@
     </row>
     <row r="845" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B845" t="str">
         <f t="shared" si="57"/>
@@ -26095,7 +26125,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueeditUserProfile</v>
       </c>
       <c r="D845" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E845" t="s">
         <v>91</v>
@@ -26115,7 +26145,7 @@
     </row>
     <row r="846" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B846" t="str">
         <f t="shared" si="57"/>
@@ -26126,7 +26156,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuesendUserEmail</v>
       </c>
       <c r="D846" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E846" t="s">
         <v>91</v>
@@ -26146,7 +26176,7 @@
     </row>
     <row r="847" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B847" t="str">
         <f t="shared" si="57"/>
@@ -26157,7 +26187,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueremove_from_team</v>
       </c>
       <c r="D847" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E847" t="s">
         <v>91</v>
@@ -26177,7 +26207,7 @@
     </row>
     <row r="848" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B848" t="str">
         <f t="shared" si="57"/>
@@ -26188,7 +26218,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueassigned_claimed_cases_plus</v>
       </c>
       <c r="D848" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E848" t="s">
         <v>15</v>
@@ -26208,7 +26238,7 @@
     </row>
     <row r="849" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A849" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B849" t="str">
         <f t="shared" si="57"/>
@@ -26219,7 +26249,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueremove_from_team2</v>
       </c>
       <c r="D849" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E849" t="s">
         <v>15</v>
@@ -26239,7 +26269,7 @@
     </row>
     <row r="850" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B850" t="str">
         <f t="shared" si="57"/>
@@ -26250,7 +26280,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuemap_view</v>
       </c>
       <c r="D850" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E850" t="s">
         <v>93</v>
@@ -26270,7 +26300,7 @@
     </row>
     <row r="851" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B851" t="str">
         <f t="shared" si="57"/>
@@ -26281,7 +26311,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuetable_view</v>
       </c>
       <c r="D851" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E851" t="s">
         <v>93</v>
@@ -26301,7 +26331,7 @@
     </row>
     <row r="852" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A852" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B852" t="str">
         <f t="shared" si="57"/>
@@ -26312,7 +26342,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueworksite</v>
       </c>
       <c r="D852" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E852" t="s">
         <v>268</v>
@@ -26332,7 +26362,7 @@
     </row>
     <row r="853" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B853" t="str">
         <f t="shared" si="57"/>
@@ -26343,7 +26373,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueworksite_details</v>
       </c>
       <c r="D853" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="E853" t="s">
         <v>69</v>
@@ -26363,7 +26393,7 @@
     </row>
     <row r="854" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B854" t="str">
         <f t="shared" si="57"/>
@@ -26374,7 +26404,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueworkTypeStatus</v>
       </c>
       <c r="D854" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E854" t="s">
         <v>87</v>
@@ -26394,7 +26424,7 @@
     </row>
     <row r="855" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B855" t="str">
         <f t="shared" si="57"/>
@@ -26425,7 +26455,7 @@
     </row>
     <row r="856" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B856" t="str">
         <f t="shared" si="57"/>
@@ -26436,7 +26466,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueteams.settings2</v>
       </c>
       <c r="D856" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E856" t="s">
         <v>93</v>
@@ -26456,7 +26486,7 @@
     </row>
     <row r="857" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B857" t="str">
         <f t="shared" si="57"/>
@@ -26467,7 +26497,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueremove_from_team3</v>
       </c>
       <c r="D857" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E857" t="s">
         <v>15</v>
@@ -26487,7 +26517,7 @@
     </row>
     <row r="858" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B858" t="str">
         <f t="shared" si="57"/>
@@ -26498,7 +26528,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuemap_view2</v>
       </c>
       <c r="D858" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E858" t="s">
         <v>92</v>
@@ -26518,7 +26548,7 @@
     </row>
     <row r="859" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A859" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B859" t="str">
         <f t="shared" si="57"/>
@@ -26529,7 +26559,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueteams.notes</v>
       </c>
       <c r="D859" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E859" t="s">
         <v>68</v>
@@ -26549,7 +26579,7 @@
     </row>
     <row r="860" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B860" t="str">
         <f t="shared" si="57"/>
@@ -26560,7 +26590,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuemembers</v>
       </c>
       <c r="D860" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E860" t="s">
         <v>98</v>
@@ -26580,7 +26610,7 @@
     </row>
     <row r="861" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B861" t="str">
         <f t="shared" si="57"/>
@@ -26591,7 +26621,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuechoose_members</v>
       </c>
       <c r="D861" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E861" t="s">
         <v>216</v>
@@ -26611,7 +26641,7 @@
     </row>
     <row r="862" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B862" t="str">
         <f t="shared" si="57"/>
@@ -26622,7 +26652,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueuser_results</v>
       </c>
       <c r="D862" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E862" t="s">
         <v>69</v>
@@ -26642,7 +26672,7 @@
     </row>
     <row r="863" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B863" t="str">
         <f t="shared" si="57"/>
@@ -26653,7 +26683,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueselect_user</v>
       </c>
       <c r="D863" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E863" t="s">
         <v>66</v>
@@ -26673,7 +26703,7 @@
     </row>
     <row r="864" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B864" t="str">
         <f t="shared" si="57"/>
@@ -26704,7 +26734,7 @@
     </row>
     <row r="865" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B865" t="str">
         <f t="shared" si="57"/>
@@ -26715,7 +26745,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueadd</v>
       </c>
       <c r="D865" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E865" t="s">
         <v>15</v>
@@ -26735,7 +26765,7 @@
     </row>
     <row r="866" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B866" t="str">
         <f t="shared" si="57"/>
@@ -26746,7 +26776,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueAddCases</v>
       </c>
       <c r="D866" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E866" t="s">
         <v>98</v>
@@ -26766,7 +26796,7 @@
     </row>
     <row r="867" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B867" t="str">
         <f t="shared" si="57"/>
@@ -26777,7 +26807,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuework_type_map</v>
       </c>
       <c r="D867" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E867" t="s">
         <v>69</v>
@@ -26797,7 +26827,7 @@
     </row>
     <row r="868" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B868" t="str">
         <f t="shared" si="57"/>
@@ -26828,7 +26858,7 @@
     </row>
     <row r="869" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B869" t="str">
         <f t="shared" si="57"/>
@@ -26839,7 +26869,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueassignable_worksite_detail</v>
       </c>
       <c r="D869" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E869" t="s">
         <v>69</v>
@@ -26859,7 +26889,7 @@
     </row>
     <row r="870" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B870" t="str">
         <f t="shared" si="57"/>
@@ -26870,7 +26900,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueassignable_worksite</v>
       </c>
       <c r="D870" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E870" t="s">
         <v>66</v>
@@ -26890,7 +26920,7 @@
     </row>
     <row r="871" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B871" t="str">
         <f t="shared" si="57"/>
@@ -26901,7 +26931,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuework_type_list</v>
       </c>
       <c r="D871" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E871" t="s">
         <v>69</v>
@@ -26921,7 +26951,7 @@
     </row>
     <row r="872" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B872" t="str">
         <f t="shared" si="57"/>
@@ -26932,7 +26962,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuework_type_dropdown</v>
       </c>
       <c r="D872" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E872" t="s">
         <v>87</v>
@@ -26952,7 +26982,7 @@
     </row>
     <row r="873" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A873" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B873" t="str">
         <f t="shared" si="57"/>
@@ -26963,7 +26993,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuecancel2</v>
       </c>
       <c r="D873" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E873" t="s">
         <v>15</v>
@@ -26983,7 +27013,7 @@
     </row>
     <row r="874" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A874" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B874" t="str">
         <f t="shared" si="57"/>
@@ -26994,7 +27024,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueaddCases2</v>
       </c>
       <c r="D874" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E874" t="s">
         <v>15</v>
@@ -27014,7 +27044,7 @@
     </row>
     <row r="875" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B875" t="str">
         <f t="shared" si="57"/>
@@ -27025,7 +27055,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vuerename_team2</v>
       </c>
       <c r="D875" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E875" t="s">
         <v>98</v>
@@ -27045,7 +27075,7 @@
     </row>
     <row r="876" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A876" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B876" t="str">
         <f t="shared" si="57"/>
@@ -27056,7 +27086,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\TeamDetail.vueteams.name</v>
       </c>
       <c r="D876" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E876" t="s">
         <v>68</v>
@@ -27076,7 +27106,7 @@
     </row>
     <row r="877" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B877" t="str">
         <f t="shared" si="57"/>
@@ -27087,7 +27117,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserEditModal.vueuser_edit</v>
       </c>
       <c r="D877" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="E877" t="s">
         <v>98</v>
@@ -27107,7 +27137,7 @@
     </row>
     <row r="878" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B878" t="str">
         <f t="shared" si="57"/>
@@ -27118,7 +27148,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserEditModal.vueprofile_picture</v>
       </c>
       <c r="D878" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E878" t="s">
         <v>93</v>
@@ -27138,7 +27168,7 @@
     </row>
     <row r="879" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B879" t="str">
         <f t="shared" si="57"/>
@@ -27169,7 +27199,7 @@
     </row>
     <row r="880" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B880" t="str">
         <f t="shared" si="57"/>
@@ -27200,7 +27230,7 @@
     </row>
     <row r="881" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A881" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B881" t="str">
         <f t="shared" si="57"/>
@@ -27231,7 +27261,7 @@
     </row>
     <row r="882" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A882" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B882" t="str">
         <f t="shared" si="57"/>
@@ -27262,7 +27292,7 @@
     </row>
     <row r="883" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A883" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B883" t="str">
         <f t="shared" si="57"/>
@@ -27293,7 +27323,7 @@
     </row>
     <row r="884" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A884" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B884" t="str">
         <f t="shared" si="57"/>
@@ -27322,9 +27352,9 @@
         <v>:data-testid="`testSave${}Button`"</v>
       </c>
     </row>
-    <row r="885" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="885" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A885" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B885" t="str">
         <f t="shared" si="57"/>
@@ -27335,7 +27365,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser</v>
       </c>
       <c r="D885" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E885" t="s">
         <v>216</v>
@@ -27353,9 +27383,9 @@
         <v>:data-testid="`testUser${}Search`"</v>
       </c>
     </row>
-    <row r="886" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A886" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B886" t="str">
         <f t="shared" ref="B886:B949" si="62">IF(A886="","",MID(A886,FIND("@",SUBSTITUTE(A886,"\","@",LEN(A886)-LEN(SUBSTITUTE(A886,"\",""))))+1,LEN(A886)))</f>
@@ -27366,7 +27396,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser_filters</v>
       </c>
       <c r="D886" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E886" t="s">
         <v>69</v>
@@ -27384,9 +27414,9 @@
         <v>:data-testid="`testUserFilters${}Div`"</v>
       </c>
     </row>
-    <row r="887" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="887" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A887" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B887" t="str">
         <f t="shared" si="62"/>
@@ -27397,7 +27427,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vuefilter_role</v>
       </c>
       <c r="D887" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E887" t="s">
         <v>69</v>
@@ -27415,9 +27445,9 @@
         <v>:data-testid="`testFilterRole${}Div`"</v>
       </c>
     </row>
-    <row r="888" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="888" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A888" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B888" t="str">
         <f t="shared" si="62"/>
@@ -27428,7 +27458,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vuefilter_invited_by</v>
       </c>
       <c r="D888" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E888" t="s">
         <v>69</v>
@@ -27446,9 +27476,9 @@
         <v>:data-testid="`testFilterInvitedBy${}Div`"</v>
       </c>
     </row>
-    <row r="889" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="889" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A889" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B889" t="str">
         <f t="shared" si="62"/>
@@ -27459,7 +27489,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser_role</v>
       </c>
       <c r="D889" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E889" t="s">
         <v>66</v>
@@ -27477,9 +27507,9 @@
         <v>:data-testid="`testUserRole${}Checkbox`"</v>
       </c>
     </row>
-    <row r="890" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="890" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A890" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B890" t="str">
         <f t="shared" si="62"/>
@@ -27509,9 +27539,9 @@
         <v>:data-testid="`test:SeveralCalculated${}`"</v>
       </c>
     </row>
-    <row r="891" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A891" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B891" t="str">
         <f t="shared" si="62"/>
@@ -27522,7 +27552,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser_invited_by</v>
       </c>
       <c r="D891" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="E891" t="s">
         <v>216</v>
@@ -27540,9 +27570,9 @@
         <v>:data-testid="`testUserInvitedBy${}Search`"</v>
       </c>
     </row>
-    <row r="892" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B892" t="str">
         <f t="shared" si="62"/>
@@ -27553,7 +27583,7 @@
         <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser_invited_by_results</v>
       </c>
       <c r="D892" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E892" t="s">
         <v>69</v>
@@ -27571,360 +27601,393 @@
         <v>:data-testid="`testUserInvitedByResults${}Div`"</v>
       </c>
     </row>
-    <row r="893" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
-        <v>743</v>
+        <v>850</v>
       </c>
       <c r="B893" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>Users.vue</v>
       </c>
       <c r="C893" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E893" t="str">
-        <f>IF(COUNTIF(C$2:C892,C893)&gt;0,"Button","")</f>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser</v>
+      </c>
+      <c r="D893" t="s">
+        <v>851</v>
+      </c>
+      <c r="E893" t="s">
+        <v>268</v>
       </c>
       <c r="F893" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testUserTable</v>
       </c>
       <c r="G893" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testUserTable"</v>
       </c>
       <c r="H893" t="str">
         <f t="shared" si="58"/>
-        <v/>
-      </c>
-    </row>
-    <row r="894" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testUser${}Table`"</v>
+      </c>
+    </row>
+    <row r="894" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
-        <v>743</v>
+        <v>850</v>
       </c>
       <c r="B894" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>Users.vue</v>
       </c>
       <c r="C894" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E894" t="str">
-        <f>IF(COUNTIF(C$2:C893,C894)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser_profile_picture</v>
+      </c>
+      <c r="D894" t="s">
+        <v>858</v>
+      </c>
+      <c r="E894" t="s">
+        <v>93</v>
       </c>
       <c r="F894" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testUserProfilePictureIcon</v>
       </c>
       <c r="G894" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testUserProfilePictureIcon"</v>
       </c>
       <c r="H894" t="str">
         <f t="shared" ref="H894:H957" si="63">IF(D894="","",":data-testid=""`"&amp;SUBSTITUTE(F894,E894,"")&amp;"${}"&amp;E894&amp;"`""")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="895" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testUserProfilePicture${}Icon`"</v>
+      </c>
+    </row>
+    <row r="895" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
-        <v>743</v>
+        <v>850</v>
       </c>
       <c r="B895" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>Users.vue</v>
       </c>
       <c r="C895" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E895" t="str">
-        <f>IF(COUNTIF(C$2:C894,C895)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser_email</v>
+      </c>
+      <c r="D895" t="s">
+        <v>859</v>
+      </c>
+      <c r="E895" t="s">
+        <v>69</v>
       </c>
       <c r="F895" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testUserEmailDiv</v>
       </c>
       <c r="G895" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testUserEmailDiv"</v>
       </c>
       <c r="H895" t="str">
         <f t="shared" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="896" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testUserEmail${}Div`"</v>
+      </c>
+    </row>
+    <row r="896" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
-        <v>743</v>
+        <v>850</v>
       </c>
       <c r="B896" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>Users.vue</v>
       </c>
       <c r="C896" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E896" t="str">
-        <f>IF(COUNTIF(C$2:C895,C896)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser_chat</v>
+      </c>
+      <c r="D896" t="s">
+        <v>860</v>
+      </c>
+      <c r="E896" t="s">
+        <v>93</v>
       </c>
       <c r="F896" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testUserChatIcon</v>
       </c>
       <c r="G896" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testUserChatIcon"</v>
       </c>
       <c r="H896" t="str">
         <f t="shared" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="897" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testUserChat${}Icon`"</v>
+      </c>
+    </row>
+    <row r="897" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
-        <v>743</v>
+        <v>850</v>
       </c>
       <c r="B897" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>Users.vue</v>
       </c>
       <c r="C897" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E897" t="str">
-        <f>IF(COUNTIF(C$2:C896,C897)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\Users.vueuser_call</v>
+      </c>
+      <c r="D897" t="s">
+        <v>861</v>
+      </c>
+      <c r="E897" t="s">
+        <v>93</v>
       </c>
       <c r="F897" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testUserCallIcon</v>
       </c>
       <c r="G897" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testUserCallIcon"</v>
       </c>
       <c r="H897" t="str">
         <f t="shared" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="898" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testUserCall${}Icon`"</v>
+      </c>
+    </row>
+    <row r="898" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
-        <v>743</v>
+        <v>862</v>
       </c>
       <c r="B898" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>UserView.vue</v>
       </c>
       <c r="C898" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E898" t="str">
-        <f>IF(COUNTIF(C$2:C897,C898)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserView.vueuser_view</v>
+      </c>
+      <c r="D898" t="s">
+        <v>863</v>
+      </c>
+      <c r="E898" t="s">
+        <v>69</v>
       </c>
       <c r="F898" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testUserViewDiv</v>
       </c>
       <c r="G898" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testUserViewDiv"</v>
       </c>
       <c r="H898" t="str">
         <f t="shared" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="899" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testUserView${}Div`"</v>
+      </c>
+    </row>
+    <row r="899" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
-        <v>743</v>
+        <v>862</v>
       </c>
       <c r="B899" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>UserView.vue</v>
       </c>
       <c r="C899" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E899" t="str">
-        <f>IF(COUNTIF(C$2:C898,C899)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserView.vueedit</v>
+      </c>
+      <c r="D899" t="s">
+        <v>371</v>
+      </c>
+      <c r="E899" t="s">
+        <v>93</v>
       </c>
       <c r="F899" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testEditIcon</v>
       </c>
       <c r="G899" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testEditIcon"</v>
       </c>
       <c r="H899" t="str">
         <f t="shared" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="900" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testEdit${}Icon`"</v>
+      </c>
+    </row>
+    <row r="900" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
-        <v>743</v>
+        <v>862</v>
       </c>
       <c r="B900" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>UserView.vue</v>
       </c>
       <c r="C900" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E900" t="str">
-        <f>IF(COUNTIF(C$2:C899,C900)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserView.vueremove_user</v>
+      </c>
+      <c r="D900" t="s">
+        <v>864</v>
+      </c>
+      <c r="E900" t="s">
+        <v>93</v>
       </c>
       <c r="F900" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testRemoveUserIcon</v>
       </c>
       <c r="G900" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testRemoveUserIcon"</v>
       </c>
       <c r="H900" t="str">
         <f t="shared" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="901" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testRemoveUser${}Icon`"</v>
+      </c>
+    </row>
+    <row r="901" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A901" t="s">
-        <v>743</v>
+        <v>862</v>
       </c>
       <c r="B901" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>UserView.vue</v>
       </c>
       <c r="C901" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E901" t="str">
-        <f>IF(COUNTIF(C$2:C900,C901)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserView.vueprofile_picture</v>
+      </c>
+      <c r="D901" t="s">
+        <v>849</v>
+      </c>
+      <c r="E901" t="s">
+        <v>93</v>
       </c>
       <c r="F901" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testProfilePictureIcon</v>
       </c>
       <c r="G901" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testProfilePictureIcon"</v>
       </c>
       <c r="H901" t="str">
         <f t="shared" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="902" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testProfilePicture${}Icon`"</v>
+      </c>
+    </row>
+    <row r="902" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A902" t="s">
-        <v>743</v>
+        <v>862</v>
       </c>
       <c r="B902" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>UserView.vue</v>
       </c>
       <c r="C902" t="str">
         <f t="shared" si="59"/>
-        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\</v>
-      </c>
-      <c r="E902" t="str">
-        <f>IF(COUNTIF(C$2:C901,C902)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserView.vueuser_details</v>
+      </c>
+      <c r="D902" t="s">
+        <v>865</v>
+      </c>
+      <c r="E902" t="s">
+        <v>69</v>
       </c>
       <c r="F902" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testUserDetailsDiv</v>
       </c>
       <c r="G902" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testUserDetailsDiv"</v>
       </c>
       <c r="H902" t="str">
         <f t="shared" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="903" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testUserDetails${}Div`"</v>
+      </c>
+    </row>
+    <row r="903" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A903" t="s">
+        <v>862</v>
+      </c>
       <c r="B903" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>UserView.vue</v>
       </c>
       <c r="C903" t="str">
         <f t="shared" si="59"/>
-        <v/>
-      </c>
-      <c r="E903" t="str">
-        <f>IF(COUNTIF(C$2:C902,C903)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserView.vueuser_roles</v>
+      </c>
+      <c r="D903" t="s">
+        <v>866</v>
+      </c>
+      <c r="E903" t="s">
+        <v>87</v>
       </c>
       <c r="F903" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testUserRolesSelect</v>
       </c>
       <c r="G903" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testUserRolesSelect"</v>
       </c>
       <c r="H903" t="str">
         <f t="shared" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="904" spans="1:8" x14ac:dyDescent="0.25">
+        <v>:data-testid="`testUserRoles${}Select`"</v>
+      </c>
+    </row>
+    <row r="904" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A904" t="s">
+        <v>862</v>
+      </c>
       <c r="B904" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>UserView.vue</v>
       </c>
       <c r="C904" t="str">
         <f t="shared" si="59"/>
-        <v/>
-      </c>
-      <c r="E904" t="str">
-        <f>IF(COUNTIF(C$2:C903,C904)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\organization\UserView.vueuser_edit</v>
+      </c>
+      <c r="D904" t="s">
+        <v>848</v>
+      </c>
+      <c r="E904" t="s">
+        <v>98</v>
       </c>
       <c r="F904" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>testUserEditModal</v>
       </c>
       <c r="G904" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>data-testid="testUserEditModal"</v>
       </c>
       <c r="H904" t="str">
         <f t="shared" si="63"/>
-        <v/>
+        <v>:data-testid="`testUserEdit${}Modal`"</v>
       </c>
     </row>
     <row r="905" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A905" t="s">
+        <v>868</v>
+      </c>
       <c r="B905" t="str">
         <f t="shared" si="62"/>
-        <v/>
+        <v>PhoneSystem.vue</v>
       </c>
       <c r="C905" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\PhoneSystem.vue</v>
       </c>
       <c r="E905" t="str">
         <f>IF(COUNTIF(C$2:C904,C905)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F905" t="str">
         <f t="shared" si="60"/>
@@ -27940,17 +28003,20 @@
       </c>
     </row>
     <row r="906" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A906" t="s">
+        <v>867</v>
+      </c>
       <c r="B906" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="C906" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</v>
       </c>
       <c r="E906" t="str">
         <f>IF(COUNTIF(C$2:C905,C906)&gt;0,"Button","")</f>
-        <v>Button</v>
+        <v/>
       </c>
       <c r="F906" t="str">
         <f t="shared" si="60"/>
@@ -27966,13 +28032,16 @@
       </c>
     </row>
     <row r="907" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A907" t="s">
+        <v>867</v>
+      </c>
       <c r="B907" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="C907" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</v>
       </c>
       <c r="E907" t="str">
         <f>IF(COUNTIF(C$2:C906,C907)&gt;0,"Button","")</f>
@@ -27992,13 +28061,16 @@
       </c>
     </row>
     <row r="908" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A908" t="s">
+        <v>867</v>
+      </c>
       <c r="B908" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="C908" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</v>
       </c>
       <c r="E908" t="str">
         <f>IF(COUNTIF(C$2:C907,C908)&gt;0,"Button","")</f>
@@ -28018,13 +28090,16 @@
       </c>
     </row>
     <row r="909" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A909" t="s">
+        <v>867</v>
+      </c>
       <c r="B909" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="C909" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</v>
       </c>
       <c r="E909" t="str">
         <f>IF(COUNTIF(C$2:C908,C909)&gt;0,"Button","")</f>
@@ -28044,13 +28119,16 @@
       </c>
     </row>
     <row r="910" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A910" t="s">
+        <v>867</v>
+      </c>
       <c r="B910" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="C910" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</v>
       </c>
       <c r="E910" t="str">
         <f>IF(COUNTIF(C$2:C909,C910)&gt;0,"Button","")</f>
@@ -28070,13 +28148,16 @@
       </c>
     </row>
     <row r="911" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A911" t="s">
+        <v>867</v>
+      </c>
       <c r="B911" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="C911" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</v>
       </c>
       <c r="E911" t="str">
         <f>IF(COUNTIF(C$2:C910,C911)&gt;0,"Button","")</f>
@@ -28096,13 +28177,16 @@
       </c>
     </row>
     <row r="912" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A912" t="s">
+        <v>867</v>
+      </c>
       <c r="B912" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="C912" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</v>
       </c>
       <c r="E912" t="str">
         <f>IF(COUNTIF(C$2:C911,C912)&gt;0,"Button","")</f>
@@ -28121,14 +28205,17 @@
         <v/>
       </c>
     </row>
-    <row r="913" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A913" t="s">
+        <v>867</v>
+      </c>
       <c r="B913" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="C913" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</v>
       </c>
       <c r="E913" t="str">
         <f>IF(COUNTIF(C$2:C912,C913)&gt;0,"Button","")</f>
@@ -28147,14 +28234,17 @@
         <v/>
       </c>
     </row>
-    <row r="914" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A914" t="s">
+        <v>867</v>
+      </c>
       <c r="B914" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="C914" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>C:\Users\Aaron\Documents\GitHub\crisiscleanup-4-web\src\pages\phone\</v>
       </c>
       <c r="E914" t="str">
         <f>IF(COUNTIF(C$2:C913,C914)&gt;0,"Button","")</f>
@@ -28173,7 +28263,7 @@
         <v/>
       </c>
     </row>
-    <row r="915" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B915" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28199,7 +28289,7 @@
         <v/>
       </c>
     </row>
-    <row r="916" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B916" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28225,7 +28315,7 @@
         <v/>
       </c>
     </row>
-    <row r="917" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B917" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28251,7 +28341,7 @@
         <v/>
       </c>
     </row>
-    <row r="918" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B918" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28277,7 +28367,7 @@
         <v/>
       </c>
     </row>
-    <row r="919" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B919" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28303,7 +28393,7 @@
         <v/>
       </c>
     </row>
-    <row r="920" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="920" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B920" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28329,7 +28419,7 @@
         <v/>
       </c>
     </row>
-    <row r="921" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B921" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28355,7 +28445,7 @@
         <v/>
       </c>
     </row>
-    <row r="922" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B922" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28381,7 +28471,7 @@
         <v/>
       </c>
     </row>
-    <row r="923" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B923" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28407,7 +28497,7 @@
         <v/>
       </c>
     </row>
-    <row r="924" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B924" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28433,7 +28523,7 @@
         <v/>
       </c>
     </row>
-    <row r="925" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B925" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28459,7 +28549,7 @@
         <v/>
       </c>
     </row>
-    <row r="926" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B926" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28485,7 +28575,7 @@
         <v/>
       </c>
     </row>
-    <row r="927" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B927" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -28511,7 +28601,7 @@
         <v/>
       </c>
     </row>
-    <row r="928" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B928" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -30549,7 +30639,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>